<commit_message>
updates 12/24/2023 20:57:06 增加字段
</commit_message>
<xml_diff>
--- a/sdk2apk.xlsx
+++ b/sdk2apk.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E103"/>
+  <dimension ref="A1:P117"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -459,145 +459,295 @@
           <t>GA</t>
         </is>
       </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>ad4screen</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>jiubang</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>Kissmetrics</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>Mixpanel</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>Heap</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>GrowingIO</t>
+        </is>
+      </c>
+      <c r="L1" s="1" t="inlineStr">
+        <is>
+          <t>Sensors</t>
+        </is>
+      </c>
+      <c r="M1" s="1" t="inlineStr">
+        <is>
+          <t>Baidu</t>
+        </is>
+      </c>
+      <c r="N1" s="1" t="inlineStr">
+        <is>
+          <t>Talkingdata</t>
+        </is>
+      </c>
+      <c r="O1" s="1" t="inlineStr">
+        <is>
+          <t>Zhuge</t>
+        </is>
+      </c>
+      <c r="P1" s="1" t="inlineStr">
+        <is>
+          <t>Amplitude</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>com.truedian.world</t>
+          <t>com.zjw.guozhifeng</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>com.tkl.fitup</t>
+          <t>com.youmoblie.opencard</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>com.topstcn.eq</t>
+          <t>cat.gencat.mobi.sem</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>com.fgl.adrianmarik.hiddenobjectrosewoodhotel2free</t>
+          <t>Repare For Kawasaki ZX10R (par_1.0.0_apkcombo.com (1)</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>com.changdu.stories</t>
-        </is>
-      </c>
+          <t>com.gau.go.launcherex.theme.ColorNeon</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>cat.gencat.mobi.acc</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>com.gau.go.launcherex.theme.ColorNeon</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr"/>
+      <c r="I2" t="inlineStr"/>
+      <c r="J2" t="inlineStr"/>
+      <c r="K2" t="inlineStr"/>
+      <c r="L2" t="inlineStr"/>
+      <c r="M2" t="inlineStr"/>
+      <c r="N2" t="inlineStr"/>
+      <c r="O2" t="inlineStr"/>
+      <c r="P2" t="inlineStr"/>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>com.wz.idphoto.idphotoproCN</t>
+          <t>com.zjw.enjoyfit</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>com.youmoblie.opencard</t>
+          <t>com.tkl.fitup</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>com.youmoblie.opencard</t>
+          <t>Wikipedia_2.7.50458-r-2023-11-09_apkcombo.com</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>com.evgenhik161.ManualeRepareForKawasakiZX10R</t>
+          <t>com.ferhapp.roastyourselfconunafrase</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>com.evgenhik161.ManualeRepareForKawasakiZX10R</t>
-        </is>
-      </c>
+          <t>Yahoo News_ Breaking &amp; Local_49.1_apkcombo.com</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>com.audaxis.mobile.voixdessports</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>com.gau.go.launcherex.theme.DarkForge</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr"/>
+      <c r="I3" t="inlineStr"/>
+      <c r="J3" t="inlineStr"/>
+      <c r="K3" t="inlineStr"/>
+      <c r="L3" t="inlineStr"/>
+      <c r="M3" t="inlineStr"/>
+      <c r="N3" t="inlineStr"/>
+      <c r="O3" t="inlineStr"/>
+      <c r="P3" t="inlineStr"/>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>com.tronlink.wallet</t>
+          <t>com.wecut.poly</t>
         </is>
       </c>
       <c r="B4" t="inlineStr"/>
       <c r="C4" t="inlineStr">
         <is>
-          <t>com.zhehekeji.hardware.zhuoyuan</t>
+          <t>com.q1.juicyhit</t>
         </is>
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>com.feridqarayev.sozoyunu</t>
+          <t>com.fgl.adrianmarik.anastasiaroseflowerprincesspremium</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>com.yousgame.MyAnimalIslandU6</t>
-        </is>
-      </c>
+          <t>com.changdu.spainreader</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>com.audaxis.mobile.sudpresse.lanouvellegazette</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>com.gau.go.launcherex.s</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr"/>
+      <c r="I4" t="inlineStr"/>
+      <c r="J4" t="inlineStr"/>
+      <c r="K4" t="inlineStr"/>
+      <c r="L4" t="inlineStr"/>
+      <c r="M4" t="inlineStr"/>
+      <c r="N4" t="inlineStr"/>
+      <c r="O4" t="inlineStr"/>
+      <c r="P4" t="inlineStr"/>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>com.wisdom.ticker</t>
+          <t>com.q1.juicyhit</t>
         </is>
       </c>
       <c r="B5" t="inlineStr"/>
       <c r="C5" t="inlineStr">
         <is>
-          <t>com.zwcode.future</t>
+          <t>TikTok_32.2.4_apkcombo.com</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>Repare For Kawasaki ZX10R (par_1.0.0_apkcombo.com (1)</t>
+          <t>com.ficamihai.logoquiz</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>com.changdu.spainreader</t>
-        </is>
-      </c>
+          <t>com.changdu.stories</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>ch.foodarena.android</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>com.gau.go.launcherex.theme.AIR.flower</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr"/>
+      <c r="I5" t="inlineStr"/>
+      <c r="J5" t="inlineStr"/>
+      <c r="K5" t="inlineStr"/>
+      <c r="L5" t="inlineStr"/>
+      <c r="M5" t="inlineStr"/>
+      <c r="N5" t="inlineStr"/>
+      <c r="O5" t="inlineStr"/>
+      <c r="P5" t="inlineStr"/>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>com.photo.in.photo.collage</t>
+          <t>com.one.vpn</t>
         </is>
       </c>
       <c r="B6" t="inlineStr"/>
       <c r="C6" t="inlineStr">
         <is>
-          <t>com.smarthome.mumbiplug</t>
+          <t>Characters+From+GOT_1.0.0_apkcombo.com</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>Which World Cup Team is This__3.2.7z_apkcombo.com</t>
+          <t>com.fgl.adrianmarik.anastasiaroseflowerprincessfree</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>com.evgenhik161.etapistroitelstva</t>
-        </is>
-      </c>
+          <t>com.gau.go.launcherex.theme.DarkForge</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>com.banquebcp.android.mobilebanking</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>com.gau.go.launcherex.theme.classic.mosaic.yhw</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr"/>
+      <c r="I6" t="inlineStr"/>
+      <c r="J6" t="inlineStr"/>
+      <c r="K6" t="inlineStr"/>
+      <c r="L6" t="inlineStr"/>
+      <c r="M6" t="inlineStr"/>
+      <c r="N6" t="inlineStr"/>
+      <c r="O6" t="inlineStr"/>
+      <c r="P6" t="inlineStr"/>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>com.youmoblie.opencard</t>
+          <t>com.wz.idphoto.idphotopro</t>
         </is>
       </c>
       <c r="B7" t="inlineStr"/>
       <c r="C7" t="inlineStr">
         <is>
-          <t>com.evgvin.feedster</t>
+          <t>com.bazarchic.android</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>com.ficamihai.logoquiz</t>
+          <t>com.evgenhik161.etapistroitelstva</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -605,155 +755,268 @@
           <t>com.ferhapp.resimkelime</t>
         </is>
       </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>com.audaxis.mobile.sudpresse.laprovince</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>com.gau.go.launcherex.gowidget.weatherwidget</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr"/>
+      <c r="I7" t="inlineStr"/>
+      <c r="J7" t="inlineStr"/>
+      <c r="K7" t="inlineStr"/>
+      <c r="L7" t="inlineStr"/>
+      <c r="M7" t="inlineStr"/>
+      <c r="N7" t="inlineStr"/>
+      <c r="O7" t="inlineStr"/>
+      <c r="P7" t="inlineStr"/>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>com.zhehekeji.hardware.zhuoyuan</t>
+          <t>com.zjw.didoband</t>
         </is>
       </c>
       <c r="B8" t="inlineStr"/>
       <c r="C8" t="inlineStr">
         <is>
-          <t>com.smartforu</t>
+          <t>com.ficamihai.logoquiz</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>com.EuSimulator</t>
+          <t>com.fgl.adrianmarik.hiddenobjectrosewoodhotel2free</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>Characters+From+GOT_1.0.0_apkcombo.com</t>
-        </is>
-      </c>
+          <t>com.gau.go.launcherex.theme.AIR.flower</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>com.audaxis.mobile.sudpresse.lacapitale</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>com.gau.go.launcherex.theme.Donahue.free</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr"/>
+      <c r="I8" t="inlineStr"/>
+      <c r="J8" t="inlineStr"/>
+      <c r="K8" t="inlineStr"/>
+      <c r="L8" t="inlineStr"/>
+      <c r="M8" t="inlineStr"/>
+      <c r="N8" t="inlineStr"/>
+      <c r="O8" t="inlineStr"/>
+      <c r="P8" t="inlineStr"/>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>com.starmiss.app</t>
+          <t>com.q1.knifesling</t>
         </is>
       </c>
       <c r="B9" t="inlineStr"/>
       <c r="C9" t="inlineStr">
         <is>
-          <t>AXS Tickets_6.1.1_apkcombo.com</t>
+          <t>com.q1.knifesling</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>com.evgenhik161.etapistroitelstva</t>
+          <t>com.ferhapp.resimkelime</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>Yahoo News_ Breaking &amp; Local_49.1_apkcombo.com</t>
-        </is>
-      </c>
+          <t>com.gau.go.launcherex.theme.classic.mosaic.yhw</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr"/>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>com.gau.go.launcherex.theme.Backup.free</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr"/>
+      <c r="I9" t="inlineStr"/>
+      <c r="J9" t="inlineStr"/>
+      <c r="K9" t="inlineStr"/>
+      <c r="L9" t="inlineStr"/>
+      <c r="M9" t="inlineStr"/>
+      <c r="N9" t="inlineStr"/>
+      <c r="O9" t="inlineStr"/>
+      <c r="P9" t="inlineStr"/>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>com.zwcode.future</t>
+          <t>com.viverify</t>
         </is>
       </c>
       <c r="B10" t="inlineStr"/>
       <c r="C10" t="inlineStr">
         <is>
-          <t>com.bgg.bgg_exchange</t>
+          <t>ch.foodarena.android</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>com.evgvin.feedster</t>
+          <t>com.fgl.adrianmarik.pinkcarservicefree</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>Repare For Kawasaki ZX10R (par_1.0.0_apkcombo.com (1)</t>
-        </is>
-      </c>
+          <t>com.gau.go.launcherex.theme.Donahue.free</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr"/>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>com.gau.go.launcherex.theme.BestThingINeverHad</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr"/>
+      <c r="I10" t="inlineStr"/>
+      <c r="J10" t="inlineStr"/>
+      <c r="K10" t="inlineStr"/>
+      <c r="L10" t="inlineStr"/>
+      <c r="M10" t="inlineStr"/>
+      <c r="N10" t="inlineStr"/>
+      <c r="O10" t="inlineStr"/>
+      <c r="P10" t="inlineStr"/>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>com.xcz.modernpoem</t>
+          <t>com.zmapp.fwatch.ald.os</t>
         </is>
       </c>
       <c r="B11" t="inlineStr"/>
       <c r="C11" t="inlineStr">
         <is>
-          <t>com.thscore.offcial</t>
+          <t>com.viverify</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>com.ferhapp.resimkelime</t>
+          <t>com.feridqarayev.sozoyunu</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>com.vivi.bed.mvp</t>
-        </is>
-      </c>
+          <t>com.q1.juicyhit</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr"/>
+      <c r="G11" t="inlineStr">
+        <is>
+          <t>com.gau.go.launcherex.theme.blackish.zt.free</t>
+        </is>
+      </c>
+      <c r="H11" t="inlineStr"/>
+      <c r="I11" t="inlineStr"/>
+      <c r="J11" t="inlineStr"/>
+      <c r="K11" t="inlineStr"/>
+      <c r="L11" t="inlineStr"/>
+      <c r="M11" t="inlineStr"/>
+      <c r="N11" t="inlineStr"/>
+      <c r="O11" t="inlineStr"/>
+      <c r="P11" t="inlineStr"/>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>com.yunkaiwulian.vglasses</t>
+          <t>com.weiou.weiou</t>
         </is>
       </c>
       <c r="B12" t="inlineStr"/>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Yahoo News_ Breaking &amp; Local_49.1_apkcombo.com</t>
+          <t>com.zmapp.fwatch.ald.os</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>com.evgenhik161.ManualeRepareForYamahaR15</t>
+          <t>Which World Cup Team is This__3.2.7z_apkcombo.com</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>Clean Master Lite - For Low-End Phones_3.1.7_apkcombo.com</t>
-        </is>
-      </c>
+          <t>com.gau.go.launcherex.theme.Color.free</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr">
+        <is>
+          <t>com.gau.go.launcherex.theme.DarkEnergy</t>
+        </is>
+      </c>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr"/>
+      <c r="J12" t="inlineStr"/>
+      <c r="K12" t="inlineStr"/>
+      <c r="L12" t="inlineStr"/>
+      <c r="M12" t="inlineStr"/>
+      <c r="N12" t="inlineStr"/>
+      <c r="O12" t="inlineStr"/>
+      <c r="P12" t="inlineStr"/>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>com.smarthome.mumbiplug</t>
+          <t>com.starmiss.app</t>
         </is>
       </c>
       <c r="B13" t="inlineStr"/>
       <c r="C13" t="inlineStr">
         <is>
-          <t>com.zhouchungame.tug</t>
+          <t>com.bestvideostudio.movieeditor</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>com.fgl.adrianmarik.anastasiaroseflowerprincesspremium</t>
+          <t>com.evgenhik161.ManualeRepareForYamahaR15</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>Avast Cleanup_23.22.0_apkcombo.com</t>
-        </is>
-      </c>
+          <t>Characters+From+GOT_1.0.0_apkcombo.com</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr"/>
+      <c r="G13" t="inlineStr">
+        <is>
+          <t>com.gau.go.launcherex.theme.ColorfulLife.flower</t>
+        </is>
+      </c>
+      <c r="H13" t="inlineStr"/>
+      <c r="I13" t="inlineStr"/>
+      <c r="J13" t="inlineStr"/>
+      <c r="K13" t="inlineStr"/>
+      <c r="L13" t="inlineStr"/>
+      <c r="M13" t="inlineStr"/>
+      <c r="N13" t="inlineStr"/>
+      <c r="O13" t="inlineStr"/>
+      <c r="P13" t="inlineStr"/>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>com.zjw.enjoyfit</t>
+          <t>com.thscore.offcial</t>
         </is>
       </c>
       <c r="B14" t="inlineStr"/>
       <c r="C14" t="inlineStr">
         <is>
-          <t>com.picooc.international</t>
+          <t>ch.davos.prototype</t>
         </is>
       </c>
       <c r="D14" t="inlineStr">
@@ -763,89 +1026,149 @@
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>com.ficamihai.logoquiz</t>
-        </is>
-      </c>
+          <t>com.ferhapp.roastyourselfconunafrase</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr"/>
+      <c r="G14" t="inlineStr">
+        <is>
+          <t>com.gau.go.launcherex.theme.Daimon.x.free</t>
+        </is>
+      </c>
+      <c r="H14" t="inlineStr"/>
+      <c r="I14" t="inlineStr"/>
+      <c r="J14" t="inlineStr"/>
+      <c r="K14" t="inlineStr"/>
+      <c r="L14" t="inlineStr"/>
+      <c r="M14" t="inlineStr"/>
+      <c r="N14" t="inlineStr"/>
+      <c r="O14" t="inlineStr"/>
+      <c r="P14" t="inlineStr"/>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>com.smartforu</t>
+          <t>com.xiaohuangtiao</t>
         </is>
       </c>
       <c r="B15" t="inlineStr"/>
       <c r="C15" t="inlineStr">
         <is>
-          <t>com.cdl.app</t>
+          <t>com.thscore.offcial</t>
         </is>
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>com.fgl.adrianmarik.pinkcarservicefree</t>
+          <t>com.evgvin.feedster</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>com.evgenhik161.ManualeRepareForYamahaR15</t>
-        </is>
-      </c>
+          <t>com.gau.go.launcherex.theme.Backup.free</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr"/>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>com.gau.go.launcherex.theme.B.and.W</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr"/>
+      <c r="I15" t="inlineStr"/>
+      <c r="J15" t="inlineStr"/>
+      <c r="K15" t="inlineStr"/>
+      <c r="L15" t="inlineStr"/>
+      <c r="M15" t="inlineStr"/>
+      <c r="N15" t="inlineStr"/>
+      <c r="O15" t="inlineStr"/>
+      <c r="P15" t="inlineStr"/>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>com.petter.swisstime_android</t>
+          <t>com.pwrd.wlwzint</t>
         </is>
       </c>
       <c r="B16" t="inlineStr"/>
       <c r="C16" t="inlineStr">
         <is>
-          <t>com.zwcode.antaivision</t>
+          <t>Chess_4.6.10-googleplay_apkcombo.com</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>com.ferhapp.roastyourselfconunafrase</t>
+          <t>com.EuSimulator</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>com.winter.scribble</t>
-        </is>
-      </c>
+          <t>com.gau.go.launcherex.theme.BestThingINeverHad</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr"/>
+      <c r="G16" t="inlineStr">
+        <is>
+          <t>com.gau.go.launcherex.theme.darkonii.free</t>
+        </is>
+      </c>
+      <c r="H16" t="inlineStr"/>
+      <c r="I16" t="inlineStr"/>
+      <c r="J16" t="inlineStr"/>
+      <c r="K16" t="inlineStr"/>
+      <c r="L16" t="inlineStr"/>
+      <c r="M16" t="inlineStr"/>
+      <c r="N16" t="inlineStr"/>
+      <c r="O16" t="inlineStr"/>
+      <c r="P16" t="inlineStr"/>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>com.videomaker.editor.slideshow.songs.record.album</t>
+          <t>com.c2s.cam</t>
         </is>
       </c>
       <c r="B17" t="inlineStr"/>
       <c r="C17" t="inlineStr">
         <is>
-          <t>com.evgenhik161.ManualeRepareForYamahaR15</t>
+          <t>com.xiaohuangtiao</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>com.fgl.adrianmarik.anastasiaroseflowerprincessfree</t>
+          <t>com.evgenhik161.ManualeRepareForKawasakiZX10R</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>com.changdu.ereader</t>
-        </is>
-      </c>
+          <t>com.ficamihai.logoquiz</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr"/>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>com.gau.go.launcherex.theme.Doodle.flower</t>
+        </is>
+      </c>
+      <c r="H17" t="inlineStr"/>
+      <c r="I17" t="inlineStr"/>
+      <c r="J17" t="inlineStr"/>
+      <c r="K17" t="inlineStr"/>
+      <c r="L17" t="inlineStr"/>
+      <c r="M17" t="inlineStr"/>
+      <c r="N17" t="inlineStr"/>
+      <c r="O17" t="inlineStr"/>
+      <c r="P17" t="inlineStr"/>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>com.bgg.bgg_exchange</t>
+          <t>com.tiqiaa.remote</t>
         </is>
       </c>
       <c r="B18" t="inlineStr"/>
       <c r="C18" t="inlineStr">
         <is>
-          <t>com.fgl.adrianmarik.pinkcarservicefree</t>
+          <t>com.pwrd.wlwzint</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
@@ -855,450 +1178,921 @@
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>Which World Cup Team is This__3.2.7z_apkcombo.com</t>
-        </is>
-      </c>
+          <t>com.gau.go.launcherex.theme.blackish.zt.free</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr"/>
+      <c r="G18" t="inlineStr">
+        <is>
+          <t>com.gau.go.launcherex.theme.Autumn.flower</t>
+        </is>
+      </c>
+      <c r="H18" t="inlineStr"/>
+      <c r="I18" t="inlineStr"/>
+      <c r="J18" t="inlineStr"/>
+      <c r="K18" t="inlineStr"/>
+      <c r="L18" t="inlineStr"/>
+      <c r="M18" t="inlineStr"/>
+      <c r="N18" t="inlineStr"/>
+      <c r="O18" t="inlineStr"/>
+      <c r="P18" t="inlineStr"/>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>com.thscore.offcial</t>
+          <t>com.truedian.world</t>
         </is>
       </c>
       <c r="B19" t="inlineStr"/>
       <c r="C19" t="inlineStr">
         <is>
-          <t>com.powervoter</t>
+          <t>com.tiqiaa.remote</t>
         </is>
       </c>
       <c r="D19" t="inlineStr"/>
       <c r="E19" t="inlineStr">
         <is>
-          <t>com.q1.knifesling</t>
-        </is>
-      </c>
+          <t>ch.foodarena.android</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr"/>
+      <c r="G19" t="inlineStr">
+        <is>
+          <t>com.gau.go.launcherex.theme.classic.free</t>
+        </is>
+      </c>
+      <c r="H19" t="inlineStr"/>
+      <c r="I19" t="inlineStr"/>
+      <c r="J19" t="inlineStr"/>
+      <c r="K19" t="inlineStr"/>
+      <c r="L19" t="inlineStr"/>
+      <c r="M19" t="inlineStr"/>
+      <c r="N19" t="inlineStr"/>
+      <c r="O19" t="inlineStr"/>
+      <c r="P19" t="inlineStr"/>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>com.youloft.calendar.almanac</t>
+          <t>com.zwcode.future</t>
         </is>
       </c>
       <c r="B20" t="inlineStr"/>
       <c r="C20" t="inlineStr">
         <is>
-          <t>com.chenyu.morepro</t>
+          <t>com.zwcode.future</t>
         </is>
       </c>
       <c r="D20" t="inlineStr"/>
       <c r="E20" t="inlineStr">
         <is>
-          <t>com.q1.juicyhit</t>
-        </is>
-      </c>
+          <t>ch.lieferservice.android</t>
+        </is>
+      </c>
+      <c r="F20" t="inlineStr"/>
+      <c r="G20" t="inlineStr">
+        <is>
+          <t>com.gau.go.launcherex.theme.Aroma.free</t>
+        </is>
+      </c>
+      <c r="H20" t="inlineStr"/>
+      <c r="I20" t="inlineStr"/>
+      <c r="J20" t="inlineStr"/>
+      <c r="K20" t="inlineStr"/>
+      <c r="L20" t="inlineStr"/>
+      <c r="M20" t="inlineStr"/>
+      <c r="N20" t="inlineStr"/>
+      <c r="O20" t="inlineStr"/>
+      <c r="P20" t="inlineStr"/>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>com.wenwen.nianfo</t>
+          <t>com.zhong.mac.fetalheartapp</t>
         </is>
       </c>
       <c r="B21" t="inlineStr"/>
       <c r="C21" t="inlineStr">
         <is>
-          <t>com.williamL</t>
+          <t>com.audaxis.nordlittoral</t>
         </is>
       </c>
       <c r="D21" t="inlineStr"/>
       <c r="E21" t="inlineStr">
         <is>
-          <t>Don't Tap The White Tile_4.0.7.5_apkcombo.com</t>
-        </is>
-      </c>
+          <t>com.q1.knifesling</t>
+        </is>
+      </c>
+      <c r="F21" t="inlineStr"/>
+      <c r="G21" t="inlineStr">
+        <is>
+          <t>com.gau.go.launcherex.theme.ChristmasS.free</t>
+        </is>
+      </c>
+      <c r="H21" t="inlineStr"/>
+      <c r="I21" t="inlineStr"/>
+      <c r="J21" t="inlineStr"/>
+      <c r="K21" t="inlineStr"/>
+      <c r="L21" t="inlineStr"/>
+      <c r="M21" t="inlineStr"/>
+      <c r="N21" t="inlineStr"/>
+      <c r="O21" t="inlineStr"/>
+      <c r="P21" t="inlineStr"/>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>com.zhouchungame.tug</t>
+          <t>com.veclink.microcomm.healthy</t>
         </is>
       </c>
       <c r="B22" t="inlineStr"/>
       <c r="C22" t="inlineStr">
         <is>
-          <t>Which World Cup Team is This__3.2.7z_apkcombo.com</t>
+          <t>com.banquebcp.android.mobilebanking</t>
         </is>
       </c>
       <c r="D22" t="inlineStr"/>
       <c r="E22" t="inlineStr">
         <is>
-          <t>com.ferhapp.roastyourselfconunafrase</t>
-        </is>
-      </c>
+          <t>com.evgenhik161.etapistroitelstva</t>
+        </is>
+      </c>
+      <c r="F22" t="inlineStr"/>
+      <c r="G22" t="inlineStr">
+        <is>
+          <t>com.gau.go.launcherex.theme.cleanxxx</t>
+        </is>
+      </c>
+      <c r="H22" t="inlineStr"/>
+      <c r="I22" t="inlineStr"/>
+      <c r="J22" t="inlineStr"/>
+      <c r="K22" t="inlineStr"/>
+      <c r="L22" t="inlineStr"/>
+      <c r="M22" t="inlineStr"/>
+      <c r="N22" t="inlineStr"/>
+      <c r="O22" t="inlineStr"/>
+      <c r="P22" t="inlineStr"/>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>com.picooc.international</t>
+          <t>com.vtrump.bios</t>
         </is>
       </c>
       <c r="B23" t="inlineStr"/>
       <c r="C23" t="inlineStr">
         <is>
-          <t>com.zmapp.fwatch.ald.os</t>
+          <t>com.zwcode.eagle</t>
         </is>
       </c>
       <c r="D23" t="inlineStr"/>
-      <c r="E23" t="inlineStr"/>
+      <c r="E23" t="inlineStr">
+        <is>
+          <t>com.gau.go.launcherex.theme.DarkEnergy</t>
+        </is>
+      </c>
+      <c r="F23" t="inlineStr"/>
+      <c r="G23" t="inlineStr">
+        <is>
+          <t>com.gau.go.launcherex.theme.AlienIntruder</t>
+        </is>
+      </c>
+      <c r="H23" t="inlineStr"/>
+      <c r="I23" t="inlineStr"/>
+      <c r="J23" t="inlineStr"/>
+      <c r="K23" t="inlineStr"/>
+      <c r="L23" t="inlineStr"/>
+      <c r="M23" t="inlineStr"/>
+      <c r="N23" t="inlineStr"/>
+      <c r="O23" t="inlineStr"/>
+      <c r="P23" t="inlineStr"/>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>com.zjw.didoband</t>
+          <t>com.zwcode.eagle</t>
         </is>
       </c>
       <c r="B24" t="inlineStr"/>
       <c r="C24" t="inlineStr">
         <is>
-          <t>TikTok_32.2.4_apkcombo.com</t>
+          <t>com.smarthome.mumbiplug</t>
         </is>
       </c>
       <c r="D24" t="inlineStr"/>
-      <c r="E24" t="inlineStr"/>
+      <c r="E24" t="inlineStr">
+        <is>
+          <t>com.vivi.bed.mvp</t>
+        </is>
+      </c>
+      <c r="F24" t="inlineStr"/>
+      <c r="G24" t="inlineStr">
+        <is>
+          <t>com.gau.go.launcherex.theme.DevilPumpkin</t>
+        </is>
+      </c>
+      <c r="H24" t="inlineStr"/>
+      <c r="I24" t="inlineStr"/>
+      <c r="J24" t="inlineStr"/>
+      <c r="K24" t="inlineStr"/>
+      <c r="L24" t="inlineStr"/>
+      <c r="M24" t="inlineStr"/>
+      <c r="N24" t="inlineStr"/>
+      <c r="O24" t="inlineStr"/>
+      <c r="P24" t="inlineStr"/>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>com.zwcode.antaivision</t>
+          <t>com.smarthome.mumbiplug</t>
         </is>
       </c>
       <c r="B25" t="inlineStr"/>
       <c r="C25" t="inlineStr">
         <is>
-          <t>com.yunmai.scaleen</t>
+          <t>Avast Cleanup_23.22.0_apkcombo.com</t>
         </is>
       </c>
       <c r="D25" t="inlineStr"/>
-      <c r="E25" t="inlineStr"/>
+      <c r="E25" t="inlineStr">
+        <is>
+          <t>ch.davos.prototype</t>
+        </is>
+      </c>
+      <c r="F25" t="inlineStr"/>
+      <c r="G25" t="inlineStr">
+        <is>
+          <t>com.gau.go.launcherex.theme.Christmas.Day</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr"/>
+      <c r="I25" t="inlineStr"/>
+      <c r="J25" t="inlineStr"/>
+      <c r="K25" t="inlineStr"/>
+      <c r="L25" t="inlineStr"/>
+      <c r="M25" t="inlineStr"/>
+      <c r="N25" t="inlineStr"/>
+      <c r="O25" t="inlineStr"/>
+      <c r="P25" t="inlineStr"/>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>com.pi.xdv360n</t>
+          <t>com.smarthome.sandt</t>
         </is>
       </c>
       <c r="B26" t="inlineStr"/>
       <c r="C26" t="inlineStr">
         <is>
-          <t>com.xiaohuangtiao</t>
+          <t>com.smarthome.sandt</t>
         </is>
       </c>
       <c r="D26" t="inlineStr"/>
-      <c r="E26" t="inlineStr"/>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>com.bgmenu.android</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr"/>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>com.gau.go.launcherex.theme.dewdrop.free</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr"/>
+      <c r="I26" t="inlineStr"/>
+      <c r="J26" t="inlineStr"/>
+      <c r="K26" t="inlineStr"/>
+      <c r="L26" t="inlineStr"/>
+      <c r="M26" t="inlineStr"/>
+      <c r="N26" t="inlineStr"/>
+      <c r="O26" t="inlineStr"/>
+      <c r="P26" t="inlineStr"/>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>com.powervoter</t>
+          <t>com.vahid.clean</t>
         </is>
       </c>
       <c r="B27" t="inlineStr"/>
       <c r="C27" t="inlineStr">
         <is>
-          <t>com.videoeditor.videomaker.photos.music.pictures</t>
+          <t>com.evgenhik161.ManualeRepareForKawasakiZX10R</t>
         </is>
       </c>
       <c r="D27" t="inlineStr"/>
-      <c r="E27" t="inlineStr"/>
+      <c r="E27" t="inlineStr">
+        <is>
+          <t>com.gau.go.launcherex.theme.ColorfulLife.flower</t>
+        </is>
+      </c>
+      <c r="F27" t="inlineStr"/>
+      <c r="G27" t="inlineStr">
+        <is>
+          <t>com.gau.go.launcherex.theme.ChristmasEve.ys</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr"/>
+      <c r="I27" t="inlineStr"/>
+      <c r="J27" t="inlineStr"/>
+      <c r="K27" t="inlineStr"/>
+      <c r="L27" t="inlineStr"/>
+      <c r="M27" t="inlineStr"/>
+      <c r="N27" t="inlineStr"/>
+      <c r="O27" t="inlineStr"/>
+      <c r="P27" t="inlineStr"/>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>com.zjw.guozhifeng</t>
+          <t>com.zwcode.p6spro</t>
         </is>
       </c>
       <c r="B28" t="inlineStr"/>
       <c r="C28" t="inlineStr">
         <is>
-          <t>com.pwrd.wlwzint</t>
+          <t>be.pizza.android</t>
         </is>
       </c>
       <c r="D28" t="inlineStr"/>
-      <c r="E28" t="inlineStr"/>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Which World Cup Team is This__3.2.7z_apkcombo.com</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr"/>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>com.gau.go.launcherex.theme.Dark.mayi</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr"/>
+      <c r="I28" t="inlineStr"/>
+      <c r="J28" t="inlineStr"/>
+      <c r="K28" t="inlineStr"/>
+      <c r="L28" t="inlineStr"/>
+      <c r="M28" t="inlineStr"/>
+      <c r="N28" t="inlineStr"/>
+      <c r="O28" t="inlineStr"/>
+      <c r="P28" t="inlineStr"/>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>com.williamL</t>
+          <t>com.wifiaudio.livaiaspeaker</t>
         </is>
       </c>
       <c r="B29" t="inlineStr"/>
       <c r="C29" t="inlineStr">
         <is>
-          <t>Chess_4.6.10-googleplay_apkcombo.com</t>
+          <t>com.audaxis.mobile.voixdessports</t>
         </is>
       </c>
       <c r="D29" t="inlineStr"/>
-      <c r="E29" t="inlineStr"/>
+      <c r="E29" t="inlineStr">
+        <is>
+          <t>Don't Tap The White Tile_4.0.7.5_apkcombo.com</t>
+        </is>
+      </c>
+      <c r="F29" t="inlineStr"/>
+      <c r="G29" t="inlineStr">
+        <is>
+          <t>com.gau.go.launcherex.theme.Ample</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr"/>
+      <c r="I29" t="inlineStr"/>
+      <c r="J29" t="inlineStr"/>
+      <c r="K29" t="inlineStr"/>
+      <c r="L29" t="inlineStr"/>
+      <c r="M29" t="inlineStr"/>
+      <c r="N29" t="inlineStr"/>
+      <c r="O29" t="inlineStr"/>
+      <c r="P29" t="inlineStr"/>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>com.zmapp.fwatch.ald.os</t>
+          <t>com.photo.in.photo.collage</t>
         </is>
       </c>
       <c r="B30" t="inlineStr"/>
       <c r="C30" t="inlineStr">
         <is>
-          <t>com.europosit.coloring</t>
+          <t>com.zwcode.p6spro</t>
         </is>
       </c>
       <c r="D30" t="inlineStr"/>
-      <c r="E30" t="inlineStr"/>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Clean Master Lite - For Low-End Phones_3.1.7_apkcombo.com</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr"/>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>com.gau.go.launcherex.theme.Color.free</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr"/>
+      <c r="I30" t="inlineStr"/>
+      <c r="J30" t="inlineStr"/>
+      <c r="K30" t="inlineStr"/>
+      <c r="L30" t="inlineStr"/>
+      <c r="M30" t="inlineStr"/>
+      <c r="N30" t="inlineStr"/>
+      <c r="O30" t="inlineStr"/>
+      <c r="P30" t="inlineStr"/>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>com.wallstreetcn.weex</t>
+          <t>com.uthink.ring.bingosport</t>
         </is>
       </c>
       <c r="B31" t="inlineStr"/>
       <c r="C31" t="inlineStr">
         <is>
-          <t>com.evgenhik161.etapistroitelstva</t>
+          <t>com.europosit.coloring</t>
         </is>
       </c>
       <c r="D31" t="inlineStr"/>
-      <c r="E31" t="inlineStr"/>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>Repare For Kawasaki ZX10R (par_1.0.0_apkcombo.com (1)</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr"/>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>com.gau.go.launcherex.theme.DarkSpeed</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr"/>
+      <c r="I31" t="inlineStr"/>
+      <c r="J31" t="inlineStr"/>
+      <c r="K31" t="inlineStr"/>
+      <c r="L31" t="inlineStr"/>
+      <c r="M31" t="inlineStr"/>
+      <c r="N31" t="inlineStr"/>
+      <c r="O31" t="inlineStr"/>
+      <c r="P31" t="inlineStr"/>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>com.yunmai.scaleen</t>
+          <t>com.careerx</t>
         </is>
       </c>
       <c r="B32" t="inlineStr"/>
       <c r="C32" t="inlineStr">
         <is>
-          <t>Characters+From+GOT_1.0.0_apkcombo.com</t>
+          <t>com.topstcn.eq</t>
         </is>
       </c>
       <c r="D32" t="inlineStr"/>
-      <c r="E32" t="inlineStr"/>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>be.rossel.lardennais</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr"/>
+      <c r="G32" t="inlineStr"/>
+      <c r="H32" t="inlineStr"/>
+      <c r="I32" t="inlineStr"/>
+      <c r="J32" t="inlineStr"/>
+      <c r="K32" t="inlineStr"/>
+      <c r="L32" t="inlineStr"/>
+      <c r="M32" t="inlineStr"/>
+      <c r="N32" t="inlineStr"/>
+      <c r="O32" t="inlineStr"/>
+      <c r="P32" t="inlineStr"/>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>com.pi.e360</t>
+          <t>com.tracebird</t>
         </is>
       </c>
       <c r="B33" t="inlineStr"/>
       <c r="C33" t="inlineStr">
         <is>
-          <t>com.zwcode.p6spro</t>
+          <t>com.xvideostudio.videoeditor</t>
         </is>
       </c>
       <c r="D33" t="inlineStr"/>
-      <c r="E33" t="inlineStr"/>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>com.audaxis.mobile.smart.union</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr"/>
+      <c r="G33" t="inlineStr"/>
+      <c r="H33" t="inlineStr"/>
+      <c r="I33" t="inlineStr"/>
+      <c r="J33" t="inlineStr"/>
+      <c r="K33" t="inlineStr"/>
+      <c r="L33" t="inlineStr"/>
+      <c r="M33" t="inlineStr"/>
+      <c r="N33" t="inlineStr"/>
+      <c r="O33" t="inlineStr"/>
+      <c r="P33" t="inlineStr"/>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>com.xiaohuangtiao</t>
+          <t>com.changdu.spainreader</t>
         </is>
       </c>
       <c r="B34" t="inlineStr"/>
       <c r="C34" t="inlineStr">
         <is>
-          <t>com.ce.gwadarpro</t>
+          <t>com.audaxis.mobile.sudpresse.lacapitale</t>
         </is>
       </c>
       <c r="D34" t="inlineStr"/>
-      <c r="E34" t="inlineStr"/>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>com.audaxis.nordlittoral</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr"/>
+      <c r="G34" t="inlineStr"/>
+      <c r="H34" t="inlineStr"/>
+      <c r="I34" t="inlineStr"/>
+      <c r="J34" t="inlineStr"/>
+      <c r="K34" t="inlineStr"/>
+      <c r="L34" t="inlineStr"/>
+      <c r="M34" t="inlineStr"/>
+      <c r="N34" t="inlineStr"/>
+      <c r="O34" t="inlineStr"/>
+      <c r="P34" t="inlineStr"/>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>com.one.vpn</t>
+          <t>com.changdu.stories</t>
         </is>
       </c>
       <c r="B35" t="inlineStr"/>
       <c r="C35" t="inlineStr">
         <is>
-          <t>com.zwcode.glenz</t>
+          <t>com.tracebird</t>
         </is>
       </c>
       <c r="D35" t="inlineStr"/>
-      <c r="E35" t="inlineStr"/>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>com.gau.go.launcherex.theme.Daimon.x.free</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr"/>
+      <c r="G35" t="inlineStr"/>
+      <c r="H35" t="inlineStr"/>
+      <c r="I35" t="inlineStr"/>
+      <c r="J35" t="inlineStr"/>
+      <c r="K35" t="inlineStr"/>
+      <c r="L35" t="inlineStr"/>
+      <c r="M35" t="inlineStr"/>
+      <c r="N35" t="inlineStr"/>
+      <c r="O35" t="inlineStr"/>
+      <c r="P35" t="inlineStr"/>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>com.perfant.eyesir.nano</t>
+          <t>com.wecut.vapor</t>
         </is>
       </c>
       <c r="B36" t="inlineStr"/>
       <c r="C36" t="inlineStr">
         <is>
-          <t>Repare For Kawasaki ZX10R (par_1.0.0_apkcombo.com (1)</t>
+          <t>com.changdu.spainreader</t>
         </is>
       </c>
       <c r="D36" t="inlineStr"/>
-      <c r="E36" t="inlineStr"/>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>com.gau.go.launcherex.theme.B.and.W</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr"/>
+      <c r="G36" t="inlineStr"/>
+      <c r="H36" t="inlineStr"/>
+      <c r="I36" t="inlineStr"/>
+      <c r="J36" t="inlineStr"/>
+      <c r="K36" t="inlineStr"/>
+      <c r="L36" t="inlineStr"/>
+      <c r="M36" t="inlineStr"/>
+      <c r="N36" t="inlineStr"/>
+      <c r="O36" t="inlineStr"/>
+      <c r="P36" t="inlineStr"/>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>com.chigo.global.android.controller.activity</t>
+          <t>com.wallstreetcn.news.googleplay</t>
         </is>
       </c>
       <c r="B37" t="inlineStr"/>
       <c r="C37" t="inlineStr">
         <is>
-          <t>Avast Cleanup_23.22.0_apkcombo.com</t>
+          <t>com.changdu.stories</t>
         </is>
       </c>
       <c r="D37" t="inlineStr"/>
-      <c r="E37" t="inlineStr"/>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>com.gau.go.launcherex.theme.darkonii.free</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr"/>
+      <c r="G37" t="inlineStr"/>
+      <c r="H37" t="inlineStr"/>
+      <c r="I37" t="inlineStr"/>
+      <c r="J37" t="inlineStr"/>
+      <c r="K37" t="inlineStr"/>
+      <c r="L37" t="inlineStr"/>
+      <c r="M37" t="inlineStr"/>
+      <c r="N37" t="inlineStr"/>
+      <c r="O37" t="inlineStr"/>
+      <c r="P37" t="inlineStr"/>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>com.youloft.calendar12</t>
+          <t>com.petter.swisstime_android</t>
         </is>
       </c>
       <c r="B38" t="inlineStr"/>
       <c r="C38" t="inlineStr">
         <is>
-          <t>com.chargespotbo.app</t>
+          <t>com.fgl.adrianmarik.pinkcarservicefree</t>
         </is>
       </c>
       <c r="D38" t="inlineStr"/>
-      <c r="E38" t="inlineStr"/>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>com.gau.go.launcherex.theme.Doodle.flower</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr"/>
+      <c r="G38" t="inlineStr"/>
+      <c r="H38" t="inlineStr"/>
+      <c r="I38" t="inlineStr"/>
+      <c r="J38" t="inlineStr"/>
+      <c r="K38" t="inlineStr"/>
+      <c r="L38" t="inlineStr"/>
+      <c r="M38" t="inlineStr"/>
+      <c r="N38" t="inlineStr"/>
+      <c r="O38" t="inlineStr"/>
+      <c r="P38" t="inlineStr"/>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>com.uthink.ring.bingosport</t>
+          <t>com.tronlink.wallet</t>
         </is>
       </c>
       <c r="B39" t="inlineStr"/>
       <c r="C39" t="inlineStr">
         <is>
-          <t>com.zwcode.vantech</t>
+          <t>com.zwcode.ateyes</t>
         </is>
       </c>
       <c r="D39" t="inlineStr"/>
-      <c r="E39" t="inlineStr"/>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>com.gau.go.launcherex.theme.Autumn.flower</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr"/>
+      <c r="G39" t="inlineStr"/>
+      <c r="H39" t="inlineStr"/>
+      <c r="I39" t="inlineStr"/>
+      <c r="J39" t="inlineStr"/>
+      <c r="K39" t="inlineStr"/>
+      <c r="L39" t="inlineStr"/>
+      <c r="M39" t="inlineStr"/>
+      <c r="N39" t="inlineStr"/>
+      <c r="O39" t="inlineStr"/>
+      <c r="P39" t="inlineStr"/>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>com.wecut.vapor</t>
+          <t>com.zwcode.ateyes</t>
         </is>
       </c>
       <c r="B40" t="inlineStr"/>
       <c r="C40" t="inlineStr">
         <is>
-          <t>Wikipedia_2.7.50458-r-2023-11-09_apkcombo.com</t>
+          <t>com.gau.go.launcherex.gowidget.weatherwidget</t>
         </is>
       </c>
       <c r="D40" t="inlineStr"/>
-      <c r="E40" t="inlineStr"/>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>Avast Cleanup_23.22.0_apkcombo.com</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr"/>
+      <c r="G40" t="inlineStr"/>
+      <c r="H40" t="inlineStr"/>
+      <c r="I40" t="inlineStr"/>
+      <c r="J40" t="inlineStr"/>
+      <c r="K40" t="inlineStr"/>
+      <c r="L40" t="inlineStr"/>
+      <c r="M40" t="inlineStr"/>
+      <c r="N40" t="inlineStr"/>
+      <c r="O40" t="inlineStr"/>
+      <c r="P40" t="inlineStr"/>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>com.pwrd.wlwzint</t>
+          <t>com.wallstreetcn.weex</t>
         </is>
       </c>
       <c r="B41" t="inlineStr"/>
       <c r="C41" t="inlineStr">
         <is>
-          <t>com.cat.simulation</t>
+          <t>com.fgl.adrianmarik.anastasiaroseflowerprincesspremium</t>
         </is>
       </c>
       <c r="D41" t="inlineStr"/>
-      <c r="E41" t="inlineStr"/>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>com.audaxis.mobile.sudpresse.laprovince</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr"/>
+      <c r="G41" t="inlineStr"/>
+      <c r="H41" t="inlineStr"/>
+      <c r="I41" t="inlineStr"/>
+      <c r="J41" t="inlineStr"/>
+      <c r="K41" t="inlineStr"/>
+      <c r="L41" t="inlineStr"/>
+      <c r="M41" t="inlineStr"/>
+      <c r="N41" t="inlineStr"/>
+      <c r="O41" t="inlineStr"/>
+      <c r="P41" t="inlineStr"/>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>com.zosi.cam</t>
+          <t>com.pancam.chamelon.nano</t>
         </is>
       </c>
       <c r="B42" t="inlineStr"/>
       <c r="C42" t="inlineStr">
         <is>
-          <t>com.q1.knifesling</t>
+          <t>com.uthink.ring</t>
         </is>
       </c>
       <c r="D42" t="inlineStr"/>
-      <c r="E42" t="inlineStr"/>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>com.evgenhik161.ManualeRepareForYamahaR15</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr"/>
+      <c r="G42" t="inlineStr"/>
+      <c r="H42" t="inlineStr"/>
+      <c r="I42" t="inlineStr"/>
+      <c r="J42" t="inlineStr"/>
+      <c r="K42" t="inlineStr"/>
+      <c r="L42" t="inlineStr"/>
+      <c r="M42" t="inlineStr"/>
+      <c r="N42" t="inlineStr"/>
+      <c r="O42" t="inlineStr"/>
+      <c r="P42" t="inlineStr"/>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>com.pancam.chamelon.nano</t>
+          <t>com.bvi.gogoapp</t>
         </is>
       </c>
       <c r="B43" t="inlineStr"/>
       <c r="C43" t="inlineStr">
         <is>
-          <t>com.FidgetSpinnerinSpace.starrapps</t>
+          <t>com.evgenhik161.etapistroitelstva</t>
         </is>
       </c>
       <c r="D43" t="inlineStr"/>
-      <c r="E43" t="inlineStr"/>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>com.gau.go.launcherex.theme.classic.free</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr"/>
+      <c r="G43" t="inlineStr"/>
+      <c r="H43" t="inlineStr"/>
+      <c r="I43" t="inlineStr"/>
+      <c r="J43" t="inlineStr"/>
+      <c r="K43" t="inlineStr"/>
+      <c r="L43" t="inlineStr"/>
+      <c r="M43" t="inlineStr"/>
+      <c r="N43" t="inlineStr"/>
+      <c r="O43" t="inlineStr"/>
+      <c r="P43" t="inlineStr"/>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>com.pi.MGC360</t>
+          <t>com.vivi.bed.mvp</t>
         </is>
       </c>
       <c r="B44" t="inlineStr"/>
       <c r="C44" t="inlineStr">
         <is>
-          <t>com.changdu.stories</t>
+          <t>cat.gencat.mobi.airecat</t>
         </is>
       </c>
       <c r="D44" t="inlineStr"/>
-      <c r="E44" t="inlineStr"/>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>com.gau.go.launcherex.theme.Aroma.free</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr"/>
+      <c r="G44" t="inlineStr"/>
+      <c r="H44" t="inlineStr"/>
+      <c r="I44" t="inlineStr"/>
+      <c r="J44" t="inlineStr"/>
+      <c r="K44" t="inlineStr"/>
+      <c r="L44" t="inlineStr"/>
+      <c r="M44" t="inlineStr"/>
+      <c r="N44" t="inlineStr"/>
+      <c r="O44" t="inlineStr"/>
+      <c r="P44" t="inlineStr"/>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>com.zevercloud.app.pushmessage</t>
+          <t>com.youloft.calendar12</t>
         </is>
       </c>
       <c r="B45" t="inlineStr"/>
       <c r="C45" t="inlineStr">
         <is>
-          <t>com.centaline.centalinemacau</t>
+          <t>com.europosit.pixelcoloring</t>
         </is>
       </c>
       <c r="D45" t="inlineStr"/>
-      <c r="E45" t="inlineStr"/>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>com.gau.go.launcherex.theme.AlienIntruder</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr"/>
+      <c r="G45" t="inlineStr"/>
+      <c r="H45" t="inlineStr"/>
+      <c r="I45" t="inlineStr"/>
+      <c r="J45" t="inlineStr"/>
+      <c r="K45" t="inlineStr"/>
+      <c r="L45" t="inlineStr"/>
+      <c r="M45" t="inlineStr"/>
+      <c r="N45" t="inlineStr"/>
+      <c r="O45" t="inlineStr"/>
+      <c r="P45" t="inlineStr"/>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>com.zwcode.p6spro</t>
+          <t>com.zosi.cam</t>
         </is>
       </c>
       <c r="B46" t="inlineStr"/>
       <c r="C46" t="inlineStr">
         <is>
-          <t>com.changdu.spainreader</t>
+          <t>com.vivi.bed.mvp</t>
         </is>
       </c>
       <c r="D46" t="inlineStr"/>
-      <c r="E46" t="inlineStr"/>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>com.evgenhik161.ManualeRepareForKawasakiZX10R</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr"/>
+      <c r="G46" t="inlineStr"/>
+      <c r="H46" t="inlineStr"/>
+      <c r="I46" t="inlineStr"/>
+      <c r="J46" t="inlineStr"/>
+      <c r="K46" t="inlineStr"/>
+      <c r="L46" t="inlineStr"/>
+      <c r="M46" t="inlineStr"/>
+      <c r="N46" t="inlineStr"/>
+      <c r="O46" t="inlineStr"/>
+      <c r="P46" t="inlineStr"/>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>com.zwcode.glenz</t>
+          <t>com.xcz.modernpoem</t>
         </is>
       </c>
       <c r="B47" t="inlineStr"/>
@@ -1308,688 +2102,1312 @@
         </is>
       </c>
       <c r="D47" t="inlineStr"/>
-      <c r="E47" t="inlineStr"/>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>com.gau.go.launcherex.theme.ChristmasS.free</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr"/>
+      <c r="G47" t="inlineStr"/>
+      <c r="H47" t="inlineStr"/>
+      <c r="I47" t="inlineStr"/>
+      <c r="J47" t="inlineStr"/>
+      <c r="K47" t="inlineStr"/>
+      <c r="L47" t="inlineStr"/>
+      <c r="M47" t="inlineStr"/>
+      <c r="N47" t="inlineStr"/>
+      <c r="O47" t="inlineStr"/>
+      <c r="P47" t="inlineStr"/>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>com.bvi.gogoapp</t>
+          <t>com.zwcode.vantech</t>
         </is>
       </c>
       <c r="B48" t="inlineStr"/>
       <c r="C48" t="inlineStr">
         <is>
-          <t>com.viverify</t>
+          <t>AXS Tickets_6.1.1_apkcombo.com</t>
         </is>
       </c>
       <c r="D48" t="inlineStr"/>
-      <c r="E48" t="inlineStr"/>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>be.pizza.android</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr"/>
+      <c r="G48" t="inlineStr"/>
+      <c r="H48" t="inlineStr"/>
+      <c r="I48" t="inlineStr"/>
+      <c r="J48" t="inlineStr"/>
+      <c r="K48" t="inlineStr"/>
+      <c r="L48" t="inlineStr"/>
+      <c r="M48" t="inlineStr"/>
+      <c r="N48" t="inlineStr"/>
+      <c r="O48" t="inlineStr"/>
+      <c r="P48" t="inlineStr"/>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>com.chargespotbo.app</t>
+          <t>com.zwcode.glenz</t>
         </is>
       </c>
       <c r="B49" t="inlineStr"/>
       <c r="C49" t="inlineStr">
         <is>
-          <t>com.x10_linked.cam</t>
+          <t>com.zwcode.vantech</t>
         </is>
       </c>
       <c r="D49" t="inlineStr"/>
-      <c r="E49" t="inlineStr"/>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>com.accor.appli.hybrid</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr"/>
+      <c r="G49" t="inlineStr"/>
+      <c r="H49" t="inlineStr"/>
+      <c r="I49" t="inlineStr"/>
+      <c r="J49" t="inlineStr"/>
+      <c r="K49" t="inlineStr"/>
+      <c r="L49" t="inlineStr"/>
+      <c r="M49" t="inlineStr"/>
+      <c r="N49" t="inlineStr"/>
+      <c r="O49" t="inlineStr"/>
+      <c r="P49" t="inlineStr"/>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>com.vordon.cam</t>
+          <t>com.peake.cleaner</t>
         </is>
       </c>
       <c r="B50" t="inlineStr"/>
       <c r="C50" t="inlineStr">
         <is>
-          <t>com.ferhapp.resimkelime</t>
+          <t>Which World Cup Team is This__3.2.7z_apkcombo.com</t>
         </is>
       </c>
       <c r="D50" t="inlineStr"/>
-      <c r="E50" t="inlineStr"/>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>com.audaxis.mobile.voixdessports</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr"/>
+      <c r="G50" t="inlineStr"/>
+      <c r="H50" t="inlineStr"/>
+      <c r="I50" t="inlineStr"/>
+      <c r="J50" t="inlineStr"/>
+      <c r="K50" t="inlineStr"/>
+      <c r="L50" t="inlineStr"/>
+      <c r="M50" t="inlineStr"/>
+      <c r="N50" t="inlineStr"/>
+      <c r="O50" t="inlineStr"/>
+      <c r="P50" t="inlineStr"/>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>com.winter.scribble</t>
+          <t>com.wz.idphoto.idphotoproCN</t>
         </is>
       </c>
       <c r="B51" t="inlineStr"/>
       <c r="C51" t="inlineStr">
         <is>
-          <t>com.zwcode.uptech</t>
+          <t>com.zwcode.glenz</t>
         </is>
       </c>
       <c r="D51" t="inlineStr"/>
-      <c r="E51" t="inlineStr"/>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>com.gau.go.launcherex.theme.DevilPumpkin</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr"/>
+      <c r="G51" t="inlineStr"/>
+      <c r="H51" t="inlineStr"/>
+      <c r="I51" t="inlineStr"/>
+      <c r="J51" t="inlineStr"/>
+      <c r="K51" t="inlineStr"/>
+      <c r="L51" t="inlineStr"/>
+      <c r="M51" t="inlineStr"/>
+      <c r="N51" t="inlineStr"/>
+      <c r="O51" t="inlineStr"/>
+      <c r="P51" t="inlineStr"/>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>com.zwcode.vantech</t>
+          <t>com.cem.leyubaby.foreign</t>
         </is>
       </c>
       <c r="B52" t="inlineStr"/>
       <c r="C52" t="inlineStr">
         <is>
-          <t>com.bs.feifubao</t>
+          <t>com.peake.cleaner</t>
         </is>
       </c>
       <c r="D52" t="inlineStr"/>
-      <c r="E52" t="inlineStr"/>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>com.audaxis.mobile.sudpresse.lanouvellegazette</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr"/>
+      <c r="G52" t="inlineStr"/>
+      <c r="H52" t="inlineStr"/>
+      <c r="I52" t="inlineStr"/>
+      <c r="J52" t="inlineStr"/>
+      <c r="K52" t="inlineStr"/>
+      <c r="L52" t="inlineStr"/>
+      <c r="M52" t="inlineStr"/>
+      <c r="N52" t="inlineStr"/>
+      <c r="O52" t="inlineStr"/>
+      <c r="P52" t="inlineStr"/>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>com.cem.leyubaby.foreign</t>
+          <t>com.yunkaiwulian.vglasses</t>
         </is>
       </c>
       <c r="B53" t="inlineStr"/>
       <c r="C53" t="inlineStr">
         <is>
-          <t>com.wakeup.weikefit</t>
+          <t>Clean Master Lite - For Low-End Phones_3.1.7_apkcombo.com</t>
         </is>
       </c>
       <c r="D53" t="inlineStr"/>
-      <c r="E53" t="inlineStr"/>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>com.gau.go.launcherex.theme.Christmas.Day</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr"/>
+      <c r="G53" t="inlineStr"/>
+      <c r="H53" t="inlineStr"/>
+      <c r="I53" t="inlineStr"/>
+      <c r="J53" t="inlineStr"/>
+      <c r="K53" t="inlineStr"/>
+      <c r="L53" t="inlineStr"/>
+      <c r="M53" t="inlineStr"/>
+      <c r="N53" t="inlineStr"/>
+      <c r="O53" t="inlineStr"/>
+      <c r="P53" t="inlineStr"/>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>com.cat.simulation</t>
+          <t>com.yunmai.scaleen</t>
         </is>
       </c>
       <c r="B54" t="inlineStr"/>
       <c r="C54" t="inlineStr">
         <is>
-          <t>com.zwcode.lorax</t>
+          <t>com.chenyu.morepro</t>
         </is>
       </c>
       <c r="D54" t="inlineStr"/>
-      <c r="E54" t="inlineStr"/>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>com.changdu.ereader</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr"/>
+      <c r="G54" t="inlineStr"/>
+      <c r="H54" t="inlineStr"/>
+      <c r="I54" t="inlineStr"/>
+      <c r="J54" t="inlineStr"/>
+      <c r="K54" t="inlineStr"/>
+      <c r="L54" t="inlineStr"/>
+      <c r="M54" t="inlineStr"/>
+      <c r="N54" t="inlineStr"/>
+      <c r="O54" t="inlineStr"/>
+      <c r="P54" t="inlineStr"/>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>com.q1.knifesling</t>
+          <t>com.vordon.cam</t>
         </is>
       </c>
       <c r="B55" t="inlineStr"/>
       <c r="C55" t="inlineStr">
         <is>
-          <t>com.changdu.ereader</t>
+          <t>Shopify - Your Ecommerce Store_9.136.0_apkcombo.com</t>
         </is>
       </c>
       <c r="D55" t="inlineStr"/>
-      <c r="E55" t="inlineStr"/>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>com.winter.scribble</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr"/>
+      <c r="G55" t="inlineStr"/>
+      <c r="H55" t="inlineStr"/>
+      <c r="I55" t="inlineStr"/>
+      <c r="J55" t="inlineStr"/>
+      <c r="K55" t="inlineStr"/>
+      <c r="L55" t="inlineStr"/>
+      <c r="M55" t="inlineStr"/>
+      <c r="N55" t="inlineStr"/>
+      <c r="O55" t="inlineStr"/>
+      <c r="P55" t="inlineStr"/>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>com.zjw.agptek</t>
+          <t>com.powervoter</t>
         </is>
       </c>
       <c r="B56" t="inlineStr"/>
       <c r="C56" t="inlineStr">
         <is>
-          <t>com.camhr.app</t>
+          <t>com.yunmai.scaleen</t>
         </is>
       </c>
       <c r="D56" t="inlineStr"/>
-      <c r="E56" t="inlineStr"/>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>com.gau.go.launcherex.theme.dewdrop.free</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr"/>
+      <c r="G56" t="inlineStr"/>
+      <c r="H56" t="inlineStr"/>
+      <c r="I56" t="inlineStr"/>
+      <c r="J56" t="inlineStr"/>
+      <c r="K56" t="inlineStr"/>
+      <c r="L56" t="inlineStr"/>
+      <c r="M56" t="inlineStr"/>
+      <c r="N56" t="inlineStr"/>
+      <c r="O56" t="inlineStr"/>
+      <c r="P56" t="inlineStr"/>
     </row>
     <row r="57">
       <c r="A57" t="inlineStr">
         <is>
-          <t>com.veclink.microcomm.healthy</t>
+          <t>com.williamL</t>
         </is>
       </c>
       <c r="B57" t="inlineStr"/>
       <c r="C57" t="inlineStr">
         <is>
-          <t>Spotify_8.8.88.397_apkcombo.com</t>
+          <t>com.audaxis.mobile.sudpresse.laprovince</t>
         </is>
       </c>
       <c r="D57" t="inlineStr"/>
-      <c r="E57" t="inlineStr"/>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>com.gau.go.launcherex.theme.ChristmasEve.ys</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr"/>
+      <c r="G57" t="inlineStr"/>
+      <c r="H57" t="inlineStr"/>
+      <c r="I57" t="inlineStr"/>
+      <c r="J57" t="inlineStr"/>
+      <c r="K57" t="inlineStr"/>
+      <c r="L57" t="inlineStr"/>
+      <c r="M57" t="inlineStr"/>
+      <c r="N57" t="inlineStr"/>
+      <c r="O57" t="inlineStr"/>
+      <c r="P57" t="inlineStr"/>
     </row>
     <row r="58">
       <c r="A58" t="inlineStr">
         <is>
-          <t>com.changdu.stories</t>
+          <t>com.chaos.customer</t>
         </is>
       </c>
       <c r="B58" t="inlineStr"/>
       <c r="C58" t="inlineStr">
         <is>
-          <t>com.tiqiaa.remote</t>
+          <t>com.evgenhik161.ManualeRepareForYamahaR15</t>
         </is>
       </c>
       <c r="D58" t="inlineStr"/>
-      <c r="E58" t="inlineStr"/>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>com.gau.go.launcherex.theme.Dark.mayi</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr"/>
+      <c r="G58" t="inlineStr"/>
+      <c r="H58" t="inlineStr"/>
+      <c r="I58" t="inlineStr"/>
+      <c r="J58" t="inlineStr"/>
+      <c r="K58" t="inlineStr"/>
+      <c r="L58" t="inlineStr"/>
+      <c r="M58" t="inlineStr"/>
+      <c r="N58" t="inlineStr"/>
+      <c r="O58" t="inlineStr"/>
+      <c r="P58" t="inlineStr"/>
     </row>
     <row r="59">
       <c r="A59" t="inlineStr">
         <is>
-          <t>com.changdu.spainreader</t>
+          <t>com.yuedongsports.e_health</t>
         </is>
       </c>
       <c r="B59" t="inlineStr"/>
       <c r="C59" t="inlineStr">
         <is>
-          <t>com.ferhapp.roastyourselfconunafrase</t>
+          <t>com.powervoter</t>
         </is>
       </c>
       <c r="D59" t="inlineStr"/>
-      <c r="E59" t="inlineStr"/>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>com.yousgame.MyAnimalIslandU6</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr"/>
+      <c r="G59" t="inlineStr"/>
+      <c r="H59" t="inlineStr"/>
+      <c r="I59" t="inlineStr"/>
+      <c r="J59" t="inlineStr"/>
+      <c r="K59" t="inlineStr"/>
+      <c r="L59" t="inlineStr"/>
+      <c r="M59" t="inlineStr"/>
+      <c r="N59" t="inlineStr"/>
+      <c r="O59" t="inlineStr"/>
+      <c r="P59" t="inlineStr"/>
     </row>
     <row r="60">
       <c r="A60" t="inlineStr">
         <is>
-          <t>com.careerx</t>
+          <t>com.changdu.ereader</t>
         </is>
       </c>
       <c r="B60" t="inlineStr"/>
       <c r="C60" t="inlineStr">
         <is>
-          <t>com.evgenhik161.ManualeRepareForKawasakiZX10R</t>
+          <t>com.williamL</t>
         </is>
       </c>
       <c r="D60" t="inlineStr"/>
-      <c r="E60" t="inlineStr"/>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>com.audaxis.mobile.sudpresse</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr"/>
+      <c r="G60" t="inlineStr"/>
+      <c r="H60" t="inlineStr"/>
+      <c r="I60" t="inlineStr"/>
+      <c r="J60" t="inlineStr"/>
+      <c r="K60" t="inlineStr"/>
+      <c r="L60" t="inlineStr"/>
+      <c r="M60" t="inlineStr"/>
+      <c r="N60" t="inlineStr"/>
+      <c r="O60" t="inlineStr"/>
+      <c r="P60" t="inlineStr"/>
     </row>
     <row r="61">
       <c r="A61" t="inlineStr">
         <is>
-          <t>com.viverify</t>
+          <t>com.wifiac.android.controller.activity</t>
         </is>
       </c>
       <c r="B61" t="inlineStr"/>
       <c r="C61" t="inlineStr">
         <is>
-          <t>com.zwcode.orbit</t>
+          <t>com.chaos.customer</t>
         </is>
       </c>
       <c r="D61" t="inlineStr"/>
-      <c r="E61" t="inlineStr"/>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>com.gau.go.launcherex.theme.Ample</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr"/>
+      <c r="G61" t="inlineStr"/>
+      <c r="H61" t="inlineStr"/>
+      <c r="I61" t="inlineStr"/>
+      <c r="J61" t="inlineStr"/>
+      <c r="K61" t="inlineStr"/>
+      <c r="L61" t="inlineStr"/>
+      <c r="M61" t="inlineStr"/>
+      <c r="N61" t="inlineStr"/>
+      <c r="O61" t="inlineStr"/>
+      <c r="P61" t="inlineStr"/>
     </row>
     <row r="62">
       <c r="A62" t="inlineStr">
         <is>
-          <t>com.wallstreetcn.news.googleplay</t>
+          <t>com.youloft.calendar.almanac</t>
         </is>
       </c>
       <c r="B62" t="inlineStr"/>
       <c r="C62" t="inlineStr">
         <is>
-          <t>com.yunpos.neestoreapp</t>
+          <t>com.changdu.ereader</t>
         </is>
       </c>
       <c r="D62" t="inlineStr"/>
-      <c r="E62" t="inlineStr"/>
+      <c r="E62" t="inlineStr">
+        <is>
+          <t>com.gau.go.launcherex.theme.cleanxxx</t>
+        </is>
+      </c>
+      <c r="F62" t="inlineStr"/>
+      <c r="G62" t="inlineStr"/>
+      <c r="H62" t="inlineStr"/>
+      <c r="I62" t="inlineStr"/>
+      <c r="J62" t="inlineStr"/>
+      <c r="K62" t="inlineStr"/>
+      <c r="L62" t="inlineStr"/>
+      <c r="M62" t="inlineStr"/>
+      <c r="N62" t="inlineStr"/>
+      <c r="O62" t="inlineStr"/>
+      <c r="P62" t="inlineStr"/>
     </row>
     <row r="63">
       <c r="A63" t="inlineStr">
         <is>
-          <t>com.panda.catchtoy</t>
+          <t>com.zevercloud.app.pushmessage</t>
         </is>
       </c>
       <c r="B63" t="inlineStr"/>
       <c r="C63" t="inlineStr">
         <is>
-          <t>com.feridqarayev.sozoyunu</t>
+          <t>com.audaxis.mobile.sudpresse</t>
         </is>
       </c>
       <c r="D63" t="inlineStr"/>
-      <c r="E63" t="inlineStr"/>
+      <c r="E63" t="inlineStr">
+        <is>
+          <t>com.audaxis.mobile.sudpresse.lacapitale</t>
+        </is>
+      </c>
+      <c r="F63" t="inlineStr"/>
+      <c r="G63" t="inlineStr"/>
+      <c r="H63" t="inlineStr"/>
+      <c r="I63" t="inlineStr"/>
+      <c r="J63" t="inlineStr"/>
+      <c r="K63" t="inlineStr"/>
+      <c r="L63" t="inlineStr"/>
+      <c r="M63" t="inlineStr"/>
+      <c r="N63" t="inlineStr"/>
+      <c r="O63" t="inlineStr"/>
+      <c r="P63" t="inlineStr"/>
     </row>
     <row r="64">
       <c r="A64" t="inlineStr">
         <is>
-          <t>com.trinasolarhw</t>
+          <t>com.panda.catchtoy</t>
         </is>
       </c>
       <c r="B64" t="inlineStr"/>
       <c r="C64" t="inlineStr">
         <is>
-          <t>com.pets.mhcw</t>
+          <t>com.ferhapp.resimkelime</t>
         </is>
       </c>
       <c r="D64" t="inlineStr"/>
-      <c r="E64" t="inlineStr"/>
+      <c r="E64" t="inlineStr">
+        <is>
+          <t>com.gau.go.launcherex.theme.DarkSpeed</t>
+        </is>
+      </c>
+      <c r="F64" t="inlineStr"/>
+      <c r="G64" t="inlineStr"/>
+      <c r="H64" t="inlineStr"/>
+      <c r="I64" t="inlineStr"/>
+      <c r="J64" t="inlineStr"/>
+      <c r="K64" t="inlineStr"/>
+      <c r="L64" t="inlineStr"/>
+      <c r="M64" t="inlineStr"/>
+      <c r="N64" t="inlineStr"/>
+      <c r="O64" t="inlineStr"/>
+      <c r="P64" t="inlineStr"/>
     </row>
     <row r="65">
       <c r="A65" t="inlineStr">
         <is>
-          <t>com.zwcode.uptech</t>
+          <t>com.pi.e360</t>
         </is>
       </c>
       <c r="B65" t="inlineStr"/>
       <c r="C65" t="inlineStr">
         <is>
-          <t>com.wakeup.mingyuan</t>
+          <t>com.feridqarayev.sozoyunu</t>
         </is>
       </c>
       <c r="D65" t="inlineStr"/>
       <c r="E65" t="inlineStr"/>
+      <c r="F65" t="inlineStr"/>
+      <c r="G65" t="inlineStr"/>
+      <c r="H65" t="inlineStr"/>
+      <c r="I65" t="inlineStr"/>
+      <c r="J65" t="inlineStr"/>
+      <c r="K65" t="inlineStr"/>
+      <c r="L65" t="inlineStr"/>
+      <c r="M65" t="inlineStr"/>
+      <c r="N65" t="inlineStr"/>
+      <c r="O65" t="inlineStr"/>
+      <c r="P65" t="inlineStr"/>
     </row>
     <row r="66">
       <c r="A66" t="inlineStr">
         <is>
-          <t>com.orvibo.yidong</t>
+          <t>com.uthink.zitto</t>
         </is>
       </c>
       <c r="B66" t="inlineStr"/>
       <c r="C66" t="inlineStr">
         <is>
-          <t>com.youloft.lilith.en</t>
+          <t>com.zhouchungame.tug</t>
         </is>
       </c>
       <c r="D66" t="inlineStr"/>
       <c r="E66" t="inlineStr"/>
+      <c r="F66" t="inlineStr"/>
+      <c r="G66" t="inlineStr"/>
+      <c r="H66" t="inlineStr"/>
+      <c r="I66" t="inlineStr"/>
+      <c r="J66" t="inlineStr"/>
+      <c r="K66" t="inlineStr"/>
+      <c r="L66" t="inlineStr"/>
+      <c r="M66" t="inlineStr"/>
+      <c r="N66" t="inlineStr"/>
+      <c r="O66" t="inlineStr"/>
+      <c r="P66" t="inlineStr"/>
     </row>
     <row r="67">
       <c r="A67" t="inlineStr">
         <is>
-          <t>com.bs.feifubao</t>
+          <t>com.zhouchungame.tug</t>
         </is>
       </c>
       <c r="B67" t="inlineStr"/>
       <c r="C67" t="inlineStr">
         <is>
-          <t>com.wdinter.reader</t>
+          <t>com.ferhapp.roastyourselfconunafrase</t>
         </is>
       </c>
       <c r="D67" t="inlineStr"/>
       <c r="E67" t="inlineStr"/>
+      <c r="F67" t="inlineStr"/>
+      <c r="G67" t="inlineStr"/>
+      <c r="H67" t="inlineStr"/>
+      <c r="I67" t="inlineStr"/>
+      <c r="J67" t="inlineStr"/>
+      <c r="K67" t="inlineStr"/>
+      <c r="L67" t="inlineStr"/>
+      <c r="M67" t="inlineStr"/>
+      <c r="N67" t="inlineStr"/>
+      <c r="O67" t="inlineStr"/>
+      <c r="P67" t="inlineStr"/>
     </row>
     <row r="68">
       <c r="A68" t="inlineStr">
         <is>
-          <t>com.cacang.wenwan</t>
+          <t>com.bs.feifubao</t>
         </is>
       </c>
       <c r="B68" t="inlineStr"/>
       <c r="C68" t="inlineStr">
         <is>
-          <t>com.fgl.adrianmarik.anastasiaroseflowerprincessfree</t>
+          <t>com.bs.feifubao</t>
         </is>
       </c>
       <c r="D68" t="inlineStr"/>
       <c r="E68" t="inlineStr"/>
+      <c r="F68" t="inlineStr"/>
+      <c r="G68" t="inlineStr"/>
+      <c r="H68" t="inlineStr"/>
+      <c r="I68" t="inlineStr"/>
+      <c r="J68" t="inlineStr"/>
+      <c r="K68" t="inlineStr"/>
+      <c r="L68" t="inlineStr"/>
+      <c r="M68" t="inlineStr"/>
+      <c r="N68" t="inlineStr"/>
+      <c r="O68" t="inlineStr"/>
+      <c r="P68" t="inlineStr"/>
     </row>
     <row r="69">
       <c r="A69" t="inlineStr">
         <is>
-          <t>com.wakeup.weikefit</t>
+          <t>com.smartforu</t>
         </is>
       </c>
       <c r="B69" t="inlineStr"/>
       <c r="C69" t="inlineStr">
         <is>
-          <t>com.smarthome.sandt</t>
+          <t>com.smartforu</t>
         </is>
       </c>
       <c r="D69" t="inlineStr"/>
       <c r="E69" t="inlineStr"/>
+      <c r="F69" t="inlineStr"/>
+      <c r="G69" t="inlineStr"/>
+      <c r="H69" t="inlineStr"/>
+      <c r="I69" t="inlineStr"/>
+      <c r="J69" t="inlineStr"/>
+      <c r="K69" t="inlineStr"/>
+      <c r="L69" t="inlineStr"/>
+      <c r="M69" t="inlineStr"/>
+      <c r="N69" t="inlineStr"/>
+      <c r="O69" t="inlineStr"/>
+      <c r="P69" t="inlineStr"/>
     </row>
     <row r="70">
       <c r="A70" t="inlineStr">
         <is>
-          <t>com.zjw.ksixfitness</t>
+          <t>com.bgg.bgg_exchange</t>
         </is>
       </c>
       <c r="B70" t="inlineStr"/>
       <c r="C70" t="inlineStr">
         <is>
-          <t>Shopify - Your Ecommerce Store_9.136.0_apkcombo.com</t>
+          <t>com.bgg.bgg_exchange</t>
         </is>
       </c>
       <c r="D70" t="inlineStr"/>
       <c r="E70" t="inlineStr"/>
+      <c r="F70" t="inlineStr"/>
+      <c r="G70" t="inlineStr"/>
+      <c r="H70" t="inlineStr"/>
+      <c r="I70" t="inlineStr"/>
+      <c r="J70" t="inlineStr"/>
+      <c r="K70" t="inlineStr"/>
+      <c r="L70" t="inlineStr"/>
+      <c r="M70" t="inlineStr"/>
+      <c r="N70" t="inlineStr"/>
+      <c r="O70" t="inlineStr"/>
+      <c r="P70" t="inlineStr"/>
     </row>
     <row r="71">
       <c r="A71" t="inlineStr">
         <is>
-          <t>com.zwcode.lorax</t>
+          <t>com.wenwen.nianfo</t>
         </is>
       </c>
       <c r="B71" t="inlineStr"/>
       <c r="C71" t="inlineStr">
         <is>
-          <t>com.tkl.fitup</t>
+          <t>com.zwcode.lorax</t>
         </is>
       </c>
       <c r="D71" t="inlineStr"/>
       <c r="E71" t="inlineStr"/>
+      <c r="F71" t="inlineStr"/>
+      <c r="G71" t="inlineStr"/>
+      <c r="H71" t="inlineStr"/>
+      <c r="I71" t="inlineStr"/>
+      <c r="J71" t="inlineStr"/>
+      <c r="K71" t="inlineStr"/>
+      <c r="L71" t="inlineStr"/>
+      <c r="M71" t="inlineStr"/>
+      <c r="N71" t="inlineStr"/>
+      <c r="O71" t="inlineStr"/>
+      <c r="P71" t="inlineStr"/>
     </row>
     <row r="72">
       <c r="A72" t="inlineStr">
         <is>
-          <t>com.wifiaudio.livaiaspeaker</t>
+          <t>com.zwcode.lorax</t>
         </is>
       </c>
       <c r="B72" t="inlineStr"/>
       <c r="C72" t="inlineStr">
         <is>
-          <t>com.xvideostudio.videoeditor</t>
+          <t>Repare For Kawasaki ZX10R (par_1.0.0_apkcombo.com (1)</t>
         </is>
       </c>
       <c r="D72" t="inlineStr"/>
       <c r="E72" t="inlineStr"/>
+      <c r="F72" t="inlineStr"/>
+      <c r="G72" t="inlineStr"/>
+      <c r="H72" t="inlineStr"/>
+      <c r="I72" t="inlineStr"/>
+      <c r="J72" t="inlineStr"/>
+      <c r="K72" t="inlineStr"/>
+      <c r="L72" t="inlineStr"/>
+      <c r="M72" t="inlineStr"/>
+      <c r="N72" t="inlineStr"/>
+      <c r="O72" t="inlineStr"/>
+      <c r="P72" t="inlineStr"/>
     </row>
     <row r="73">
       <c r="A73" t="inlineStr">
         <is>
-          <t>com.changdu.ereader</t>
+          <t>com.perfant.eyesir.nano</t>
         </is>
       </c>
       <c r="B73" t="inlineStr"/>
       <c r="C73" t="inlineStr">
         <is>
-          <t>com.snoppa.Snoppa</t>
+          <t>cat.gencat.mobi.acc</t>
         </is>
       </c>
       <c r="D73" t="inlineStr"/>
       <c r="E73" t="inlineStr"/>
+      <c r="F73" t="inlineStr"/>
+      <c r="G73" t="inlineStr"/>
+      <c r="H73" t="inlineStr"/>
+      <c r="I73" t="inlineStr"/>
+      <c r="J73" t="inlineStr"/>
+      <c r="K73" t="inlineStr"/>
+      <c r="L73" t="inlineStr"/>
+      <c r="M73" t="inlineStr"/>
+      <c r="N73" t="inlineStr"/>
+      <c r="O73" t="inlineStr"/>
+      <c r="P73" t="inlineStr"/>
     </row>
     <row r="74">
       <c r="A74" t="inlineStr">
         <is>
-          <t>com.vtrump.bios</t>
+          <t>com.zwcode.uptech</t>
         </is>
       </c>
       <c r="B74" t="inlineStr"/>
       <c r="C74" t="inlineStr">
         <is>
-          <t>com.vivi.bed.mvp</t>
+          <t>com.zwcode.uptech</t>
         </is>
       </c>
       <c r="D74" t="inlineStr"/>
       <c r="E74" t="inlineStr"/>
+      <c r="F74" t="inlineStr"/>
+      <c r="G74" t="inlineStr"/>
+      <c r="H74" t="inlineStr"/>
+      <c r="I74" t="inlineStr"/>
+      <c r="J74" t="inlineStr"/>
+      <c r="K74" t="inlineStr"/>
+      <c r="L74" t="inlineStr"/>
+      <c r="M74" t="inlineStr"/>
+      <c r="N74" t="inlineStr"/>
+      <c r="O74" t="inlineStr"/>
+      <c r="P74" t="inlineStr"/>
     </row>
     <row r="75">
       <c r="A75" t="inlineStr">
         <is>
-          <t>com.tiqiaa.remote</t>
+          <t>com.wdinter.reader</t>
         </is>
       </c>
       <c r="B75" t="inlineStr"/>
       <c r="C75" t="inlineStr">
         <is>
-          <t>Clean Master Lite - For Low-End Phones_3.1.7_apkcombo.com</t>
+          <t>com.wdinter.reader</t>
         </is>
       </c>
       <c r="D75" t="inlineStr"/>
       <c r="E75" t="inlineStr"/>
+      <c r="F75" t="inlineStr"/>
+      <c r="G75" t="inlineStr"/>
+      <c r="H75" t="inlineStr"/>
+      <c r="I75" t="inlineStr"/>
+      <c r="J75" t="inlineStr"/>
+      <c r="K75" t="inlineStr"/>
+      <c r="L75" t="inlineStr"/>
+      <c r="M75" t="inlineStr"/>
+      <c r="N75" t="inlineStr"/>
+      <c r="O75" t="inlineStr"/>
+      <c r="P75" t="inlineStr"/>
     </row>
     <row r="76">
       <c r="A76" t="inlineStr">
         <is>
-          <t>com.wecut.poly</t>
+          <t>com.cacang.wenwan</t>
         </is>
       </c>
       <c r="B76" t="inlineStr"/>
       <c r="C76" t="inlineStr">
         <is>
-          <t>com.ficamihai.logoquiz</t>
+          <t>com.pets.mhcw</t>
         </is>
       </c>
       <c r="D76" t="inlineStr"/>
       <c r="E76" t="inlineStr"/>
+      <c r="F76" t="inlineStr"/>
+      <c r="G76" t="inlineStr"/>
+      <c r="H76" t="inlineStr"/>
+      <c r="I76" t="inlineStr"/>
+      <c r="J76" t="inlineStr"/>
+      <c r="K76" t="inlineStr"/>
+      <c r="L76" t="inlineStr"/>
+      <c r="M76" t="inlineStr"/>
+      <c r="N76" t="inlineStr"/>
+      <c r="O76" t="inlineStr"/>
+      <c r="P76" t="inlineStr"/>
     </row>
     <row r="77">
       <c r="A77" t="inlineStr">
         <is>
-          <t>com.winway.ibitcome</t>
+          <t>com.cat.simulation</t>
         </is>
       </c>
       <c r="B77" t="inlineStr"/>
       <c r="C77" t="inlineStr">
         <is>
-          <t>com.uthink.ring</t>
+          <t>cat.tv3.eng.tresac</t>
         </is>
       </c>
       <c r="D77" t="inlineStr"/>
       <c r="E77" t="inlineStr"/>
+      <c r="F77" t="inlineStr"/>
+      <c r="G77" t="inlineStr"/>
+      <c r="H77" t="inlineStr"/>
+      <c r="I77" t="inlineStr"/>
+      <c r="J77" t="inlineStr"/>
+      <c r="K77" t="inlineStr"/>
+      <c r="L77" t="inlineStr"/>
+      <c r="M77" t="inlineStr"/>
+      <c r="N77" t="inlineStr"/>
+      <c r="O77" t="inlineStr"/>
+      <c r="P77" t="inlineStr"/>
     </row>
     <row r="78">
       <c r="A78" t="inlineStr">
         <is>
-          <t>com.yousgame.MyAnimalIslandU6</t>
+          <t>com.trinasolarhw</t>
         </is>
       </c>
       <c r="B78" t="inlineStr"/>
       <c r="C78" t="inlineStr">
         <is>
-          <t>com.zwcode.eagle</t>
+          <t>com.axabanque.fr</t>
         </is>
       </c>
       <c r="D78" t="inlineStr"/>
       <c r="E78" t="inlineStr"/>
+      <c r="F78" t="inlineStr"/>
+      <c r="G78" t="inlineStr"/>
+      <c r="H78" t="inlineStr"/>
+      <c r="I78" t="inlineStr"/>
+      <c r="J78" t="inlineStr"/>
+      <c r="K78" t="inlineStr"/>
+      <c r="L78" t="inlineStr"/>
+      <c r="M78" t="inlineStr"/>
+      <c r="N78" t="inlineStr"/>
+      <c r="O78" t="inlineStr"/>
+      <c r="P78" t="inlineStr"/>
     </row>
     <row r="79">
       <c r="A79" t="inlineStr">
         <is>
-          <t>com.vahid.clean</t>
+          <t>com.zwcode.orbit</t>
         </is>
       </c>
       <c r="B79" t="inlineStr"/>
       <c r="C79" t="inlineStr">
         <is>
-          <t>com.urmet.bv.bvcloudpro</t>
+          <t>cat.catradio.eng</t>
         </is>
       </c>
       <c r="D79" t="inlineStr"/>
       <c r="E79" t="inlineStr"/>
+      <c r="F79" t="inlineStr"/>
+      <c r="G79" t="inlineStr"/>
+      <c r="H79" t="inlineStr"/>
+      <c r="I79" t="inlineStr"/>
+      <c r="J79" t="inlineStr"/>
+      <c r="K79" t="inlineStr"/>
+      <c r="L79" t="inlineStr"/>
+      <c r="M79" t="inlineStr"/>
+      <c r="N79" t="inlineStr"/>
+      <c r="O79" t="inlineStr"/>
+      <c r="P79" t="inlineStr"/>
     </row>
     <row r="80">
       <c r="A80" t="inlineStr">
         <is>
-          <t>com.wz.idphoto.idphotopro</t>
+          <t>com.zjw.agptek</t>
         </is>
       </c>
       <c r="B80" t="inlineStr"/>
       <c r="C80" t="inlineStr">
         <is>
-          <t>com.peake.cleaner</t>
+          <t>cat.gencat.mobi.home</t>
         </is>
       </c>
       <c r="D80" t="inlineStr"/>
       <c r="E80" t="inlineStr"/>
+      <c r="F80" t="inlineStr"/>
+      <c r="G80" t="inlineStr"/>
+      <c r="H80" t="inlineStr"/>
+      <c r="I80" t="inlineStr"/>
+      <c r="J80" t="inlineStr"/>
+      <c r="K80" t="inlineStr"/>
+      <c r="L80" t="inlineStr"/>
+      <c r="M80" t="inlineStr"/>
+      <c r="N80" t="inlineStr"/>
+      <c r="O80" t="inlineStr"/>
+      <c r="P80" t="inlineStr"/>
     </row>
     <row r="81">
       <c r="A81" t="inlineStr">
         <is>
-          <t>com.zwcode.orbit</t>
+          <t>com.youmoblie.opencard</t>
         </is>
       </c>
       <c r="B81" t="inlineStr"/>
       <c r="C81" t="inlineStr">
         <is>
-          <t>com.tracebird</t>
+          <t>com.cat.simulation</t>
         </is>
       </c>
       <c r="D81" t="inlineStr"/>
       <c r="E81" t="inlineStr"/>
+      <c r="F81" t="inlineStr"/>
+      <c r="G81" t="inlineStr"/>
+      <c r="H81" t="inlineStr"/>
+      <c r="I81" t="inlineStr"/>
+      <c r="J81" t="inlineStr"/>
+      <c r="K81" t="inlineStr"/>
+      <c r="L81" t="inlineStr"/>
+      <c r="M81" t="inlineStr"/>
+      <c r="N81" t="inlineStr"/>
+      <c r="O81" t="inlineStr"/>
+      <c r="P81" t="inlineStr"/>
     </row>
     <row r="82">
       <c r="A82" t="inlineStr">
         <is>
-          <t>com.yunpos.neestoreapp</t>
+          <t>com.pi.xdv360n</t>
         </is>
       </c>
       <c r="B82" t="inlineStr"/>
       <c r="C82" t="inlineStr">
         <is>
-          <t>com.zwcode.ateyes</t>
+          <t>com.zwcode.orbit</t>
         </is>
       </c>
       <c r="D82" t="inlineStr"/>
       <c r="E82" t="inlineStr"/>
+      <c r="F82" t="inlineStr"/>
+      <c r="G82" t="inlineStr"/>
+      <c r="H82" t="inlineStr"/>
+      <c r="I82" t="inlineStr"/>
+      <c r="J82" t="inlineStr"/>
+      <c r="K82" t="inlineStr"/>
+      <c r="L82" t="inlineStr"/>
+      <c r="M82" t="inlineStr"/>
+      <c r="N82" t="inlineStr"/>
+      <c r="O82" t="inlineStr"/>
+      <c r="P82" t="inlineStr"/>
     </row>
     <row r="83">
       <c r="A83" t="inlineStr">
         <is>
-          <t>com.c2s.cam</t>
+          <t>com.zjw.ksixfitness</t>
         </is>
       </c>
       <c r="B83" t="inlineStr"/>
       <c r="C83" t="inlineStr">
         <is>
-          <t>com.chaos.customer</t>
+          <t>cat.esport3.eng</t>
         </is>
       </c>
       <c r="D83" t="inlineStr"/>
       <c r="E83" t="inlineStr"/>
+      <c r="F83" t="inlineStr"/>
+      <c r="G83" t="inlineStr"/>
+      <c r="H83" t="inlineStr"/>
+      <c r="I83" t="inlineStr"/>
+      <c r="J83" t="inlineStr"/>
+      <c r="K83" t="inlineStr"/>
+      <c r="L83" t="inlineStr"/>
+      <c r="M83" t="inlineStr"/>
+      <c r="N83" t="inlineStr"/>
+      <c r="O83" t="inlineStr"/>
+      <c r="P83" t="inlineStr"/>
     </row>
     <row r="84">
       <c r="A84" t="inlineStr">
         <is>
-          <t>com.wakeup.mingyuan</t>
+          <t>com.zhehekeji.hardware.zhuoyuan</t>
         </is>
       </c>
       <c r="B84" t="inlineStr"/>
       <c r="C84" t="inlineStr">
         <is>
-          <t>com.fgl.adrianmarik.anastasiaroseflowerprincesspremium</t>
+          <t>com.cdl.app</t>
         </is>
       </c>
       <c r="D84" t="inlineStr"/>
       <c r="E84" t="inlineStr"/>
+      <c r="F84" t="inlineStr"/>
+      <c r="G84" t="inlineStr"/>
+      <c r="H84" t="inlineStr"/>
+      <c r="I84" t="inlineStr"/>
+      <c r="J84" t="inlineStr"/>
+      <c r="K84" t="inlineStr"/>
+      <c r="L84" t="inlineStr"/>
+      <c r="M84" t="inlineStr"/>
+      <c r="N84" t="inlineStr"/>
+      <c r="O84" t="inlineStr"/>
+      <c r="P84" t="inlineStr"/>
     </row>
     <row r="85">
       <c r="A85" t="inlineStr">
         <is>
-          <t>com.youloft.lilith.en</t>
+          <t>com.wakeup.mingyuan</t>
         </is>
       </c>
       <c r="B85" t="inlineStr"/>
       <c r="C85" t="inlineStr">
         <is>
-          <t>com.q1.juicyhit</t>
+          <t>com.youmoblie.opencard</t>
         </is>
       </c>
       <c r="D85" t="inlineStr"/>
       <c r="E85" t="inlineStr"/>
+      <c r="F85" t="inlineStr"/>
+      <c r="G85" t="inlineStr"/>
+      <c r="H85" t="inlineStr"/>
+      <c r="I85" t="inlineStr"/>
+      <c r="J85" t="inlineStr"/>
+      <c r="K85" t="inlineStr"/>
+      <c r="L85" t="inlineStr"/>
+      <c r="M85" t="inlineStr"/>
+      <c r="N85" t="inlineStr"/>
+      <c r="O85" t="inlineStr"/>
+      <c r="P85" t="inlineStr"/>
     </row>
     <row r="86">
       <c r="A86" t="inlineStr">
         <is>
-          <t>com.wdinter.reader</t>
+          <t>com.youloft.lilith.en</t>
         </is>
       </c>
       <c r="B86" t="inlineStr"/>
       <c r="C86" t="inlineStr">
         <is>
-          <t>com.europosit.pixelcoloring</t>
+          <t>Yahoo News_ Breaking &amp; Local_49.1_apkcombo.com</t>
         </is>
       </c>
       <c r="D86" t="inlineStr"/>
       <c r="E86" t="inlineStr"/>
+      <c r="F86" t="inlineStr"/>
+      <c r="G86" t="inlineStr"/>
+      <c r="H86" t="inlineStr"/>
+      <c r="I86" t="inlineStr"/>
+      <c r="J86" t="inlineStr"/>
+      <c r="K86" t="inlineStr"/>
+      <c r="L86" t="inlineStr"/>
+      <c r="M86" t="inlineStr"/>
+      <c r="N86" t="inlineStr"/>
+      <c r="O86" t="inlineStr"/>
+      <c r="P86" t="inlineStr"/>
     </row>
     <row r="87">
       <c r="A87" t="inlineStr">
         <is>
-          <t>com.smarthome.sandt</t>
+          <t>com.chigo.global.android.controller.activity</t>
         </is>
       </c>
       <c r="B87" t="inlineStr"/>
       <c r="C87" t="inlineStr">
         <is>
-          <t>com.zjw.wearhealth</t>
+          <t>com.zhehekeji.hardware.zhuoyuan</t>
         </is>
       </c>
       <c r="D87" t="inlineStr"/>
       <c r="E87" t="inlineStr"/>
+      <c r="F87" t="inlineStr"/>
+      <c r="G87" t="inlineStr"/>
+      <c r="H87" t="inlineStr"/>
+      <c r="I87" t="inlineStr"/>
+      <c r="J87" t="inlineStr"/>
+      <c r="K87" t="inlineStr"/>
+      <c r="L87" t="inlineStr"/>
+      <c r="M87" t="inlineStr"/>
+      <c r="N87" t="inlineStr"/>
+      <c r="O87" t="inlineStr"/>
+      <c r="P87" t="inlineStr"/>
     </row>
     <row r="88">
       <c r="A88" t="inlineStr">
         <is>
-          <t>com.yuedongsports.e_health</t>
+          <t>com.orvibo.yidong</t>
         </is>
       </c>
       <c r="B88" t="inlineStr"/>
       <c r="C88" t="inlineStr">
         <is>
-          <t>com.bestvideostudio.movieeditor</t>
+          <t>com.wakeup.mingyuan</t>
         </is>
       </c>
       <c r="D88" t="inlineStr"/>
       <c r="E88" t="inlineStr"/>
+      <c r="F88" t="inlineStr"/>
+      <c r="G88" t="inlineStr"/>
+      <c r="H88" t="inlineStr"/>
+      <c r="I88" t="inlineStr"/>
+      <c r="J88" t="inlineStr"/>
+      <c r="K88" t="inlineStr"/>
+      <c r="L88" t="inlineStr"/>
+      <c r="M88" t="inlineStr"/>
+      <c r="N88" t="inlineStr"/>
+      <c r="O88" t="inlineStr"/>
+      <c r="P88" t="inlineStr"/>
     </row>
     <row r="89">
       <c r="A89" t="inlineStr">
         <is>
-          <t>com.pi.camlink</t>
+          <t>com.pi.MGC360</t>
         </is>
       </c>
       <c r="B89" t="inlineStr"/>
-      <c r="C89" t="inlineStr"/>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>com.youloft.lilith.en</t>
+        </is>
+      </c>
       <c r="D89" t="inlineStr"/>
       <c r="E89" t="inlineStr"/>
+      <c r="F89" t="inlineStr"/>
+      <c r="G89" t="inlineStr"/>
+      <c r="H89" t="inlineStr"/>
+      <c r="I89" t="inlineStr"/>
+      <c r="J89" t="inlineStr"/>
+      <c r="K89" t="inlineStr"/>
+      <c r="L89" t="inlineStr"/>
+      <c r="M89" t="inlineStr"/>
+      <c r="N89" t="inlineStr"/>
+      <c r="O89" t="inlineStr"/>
+      <c r="P89" t="inlineStr"/>
     </row>
     <row r="90">
       <c r="A90" t="inlineStr">
         <is>
-          <t>com.uantronic.goshop3d</t>
+          <t>com.videomaker.editor.slideshow.songs.record.album</t>
         </is>
       </c>
       <c r="B90" t="inlineStr"/>
-      <c r="C90" t="inlineStr"/>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>com.gau.go.launcherex.s</t>
+        </is>
+      </c>
       <c r="D90" t="inlineStr"/>
       <c r="E90" t="inlineStr"/>
+      <c r="F90" t="inlineStr"/>
+      <c r="G90" t="inlineStr"/>
+      <c r="H90" t="inlineStr"/>
+      <c r="I90" t="inlineStr"/>
+      <c r="J90" t="inlineStr"/>
+      <c r="K90" t="inlineStr"/>
+      <c r="L90" t="inlineStr"/>
+      <c r="M90" t="inlineStr"/>
+      <c r="N90" t="inlineStr"/>
+      <c r="O90" t="inlineStr"/>
+      <c r="P90" t="inlineStr"/>
     </row>
     <row r="91">
       <c r="A91" t="inlineStr">
         <is>
-          <t>com.vivi.bed.mvp</t>
+          <t>com.chargespotbo.app</t>
         </is>
       </c>
       <c r="B91" t="inlineStr"/>
-      <c r="C91" t="inlineStr"/>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>com.wakeup.weikefit</t>
+        </is>
+      </c>
       <c r="D91" t="inlineStr"/>
       <c r="E91" t="inlineStr"/>
+      <c r="F91" t="inlineStr"/>
+      <c r="G91" t="inlineStr"/>
+      <c r="H91" t="inlineStr"/>
+      <c r="I91" t="inlineStr"/>
+      <c r="J91" t="inlineStr"/>
+      <c r="K91" t="inlineStr"/>
+      <c r="L91" t="inlineStr"/>
+      <c r="M91" t="inlineStr"/>
+      <c r="N91" t="inlineStr"/>
+      <c r="O91" t="inlineStr"/>
+      <c r="P91" t="inlineStr"/>
     </row>
     <row r="92">
       <c r="A92" t="inlineStr">
         <is>
-          <t>com.wifiac.android.controller.activity</t>
+          <t>com.yunpos.neestoreapp</t>
         </is>
       </c>
       <c r="B92" t="inlineStr"/>
-      <c r="C92" t="inlineStr"/>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>com.camhr.app</t>
+        </is>
+      </c>
       <c r="D92" t="inlineStr"/>
       <c r="E92" t="inlineStr"/>
+      <c r="F92" t="inlineStr"/>
+      <c r="G92" t="inlineStr"/>
+      <c r="H92" t="inlineStr"/>
+      <c r="I92" t="inlineStr"/>
+      <c r="J92" t="inlineStr"/>
+      <c r="K92" t="inlineStr"/>
+      <c r="L92" t="inlineStr"/>
+      <c r="M92" t="inlineStr"/>
+      <c r="N92" t="inlineStr"/>
+      <c r="O92" t="inlineStr"/>
+      <c r="P92" t="inlineStr"/>
     </row>
     <row r="93">
       <c r="A93" t="inlineStr">
         <is>
-          <t>com.zwcode.eagle</t>
+          <t>com.picooc.international</t>
         </is>
       </c>
       <c r="B93" t="inlineStr"/>
-      <c r="C93" t="inlineStr"/>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>com.chargespotbo.app</t>
+        </is>
+      </c>
       <c r="D93" t="inlineStr"/>
       <c r="E93" t="inlineStr"/>
+      <c r="F93" t="inlineStr"/>
+      <c r="G93" t="inlineStr"/>
+      <c r="H93" t="inlineStr"/>
+      <c r="I93" t="inlineStr"/>
+      <c r="J93" t="inlineStr"/>
+      <c r="K93" t="inlineStr"/>
+      <c r="L93" t="inlineStr"/>
+      <c r="M93" t="inlineStr"/>
+      <c r="N93" t="inlineStr"/>
+      <c r="O93" t="inlineStr"/>
+      <c r="P93" t="inlineStr"/>
     </row>
     <row r="94">
       <c r="A94" t="inlineStr">
         <is>
-          <t>com.uthink.zitto</t>
+          <t>Don't Tap The White Tile_4.0.7.5_apkcombo.com</t>
         </is>
       </c>
       <c r="B94" t="inlineStr"/>
-      <c r="C94" t="inlineStr"/>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>ch.lieferservice.android</t>
+        </is>
+      </c>
       <c r="D94" t="inlineStr"/>
       <c r="E94" t="inlineStr"/>
+      <c r="F94" t="inlineStr"/>
+      <c r="G94" t="inlineStr"/>
+      <c r="H94" t="inlineStr"/>
+      <c r="I94" t="inlineStr"/>
+      <c r="J94" t="inlineStr"/>
+      <c r="K94" t="inlineStr"/>
+      <c r="L94" t="inlineStr"/>
+      <c r="M94" t="inlineStr"/>
+      <c r="N94" t="inlineStr"/>
+      <c r="O94" t="inlineStr"/>
+      <c r="P94" t="inlineStr"/>
     </row>
     <row r="95">
       <c r="A95" t="inlineStr">
@@ -1998,97 +3416,540 @@
         </is>
       </c>
       <c r="B95" t="inlineStr"/>
-      <c r="C95" t="inlineStr"/>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>com.yunpos.neestoreapp</t>
+        </is>
+      </c>
       <c r="D95" t="inlineStr"/>
       <c r="E95" t="inlineStr"/>
+      <c r="F95" t="inlineStr"/>
+      <c r="G95" t="inlineStr"/>
+      <c r="H95" t="inlineStr"/>
+      <c r="I95" t="inlineStr"/>
+      <c r="J95" t="inlineStr"/>
+      <c r="K95" t="inlineStr"/>
+      <c r="L95" t="inlineStr"/>
+      <c r="M95" t="inlineStr"/>
+      <c r="N95" t="inlineStr"/>
+      <c r="O95" t="inlineStr"/>
+      <c r="P95" t="inlineStr"/>
     </row>
     <row r="96">
       <c r="A96" t="inlineStr">
         <is>
-          <t>com.peake.cleaner</t>
+          <t>com.wisdom.ticker</t>
         </is>
       </c>
       <c r="B96" t="inlineStr"/>
-      <c r="C96" t="inlineStr"/>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>com.bgmenu.android</t>
+        </is>
+      </c>
       <c r="D96" t="inlineStr"/>
       <c r="E96" t="inlineStr"/>
+      <c r="F96" t="inlineStr"/>
+      <c r="G96" t="inlineStr"/>
+      <c r="H96" t="inlineStr"/>
+      <c r="I96" t="inlineStr"/>
+      <c r="J96" t="inlineStr"/>
+      <c r="K96" t="inlineStr"/>
+      <c r="L96" t="inlineStr"/>
+      <c r="M96" t="inlineStr"/>
+      <c r="N96" t="inlineStr"/>
+      <c r="O96" t="inlineStr"/>
+      <c r="P96" t="inlineStr"/>
     </row>
     <row r="97">
       <c r="A97" t="inlineStr">
         <is>
-          <t>com.tracebird</t>
+          <t>com.winway.ibitcome</t>
         </is>
       </c>
       <c r="B97" t="inlineStr"/>
-      <c r="C97" t="inlineStr"/>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>com.picooc.international</t>
+        </is>
+      </c>
       <c r="D97" t="inlineStr"/>
       <c r="E97" t="inlineStr"/>
+      <c r="F97" t="inlineStr"/>
+      <c r="G97" t="inlineStr"/>
+      <c r="H97" t="inlineStr"/>
+      <c r="I97" t="inlineStr"/>
+      <c r="J97" t="inlineStr"/>
+      <c r="K97" t="inlineStr"/>
+      <c r="L97" t="inlineStr"/>
+      <c r="M97" t="inlineStr"/>
+      <c r="N97" t="inlineStr"/>
+      <c r="O97" t="inlineStr"/>
+      <c r="P97" t="inlineStr"/>
     </row>
     <row r="98">
       <c r="A98" t="inlineStr">
         <is>
-          <t>com.zwcode.ateyes</t>
+          <t>com.pi.camlink</t>
         </is>
       </c>
       <c r="B98" t="inlineStr"/>
-      <c r="C98" t="inlineStr"/>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>com.baracodamedia.android.rtl</t>
+        </is>
+      </c>
       <c r="D98" t="inlineStr"/>
       <c r="E98" t="inlineStr"/>
+      <c r="F98" t="inlineStr"/>
+      <c r="G98" t="inlineStr"/>
+      <c r="H98" t="inlineStr"/>
+      <c r="I98" t="inlineStr"/>
+      <c r="J98" t="inlineStr"/>
+      <c r="K98" t="inlineStr"/>
+      <c r="L98" t="inlineStr"/>
+      <c r="M98" t="inlineStr"/>
+      <c r="N98" t="inlineStr"/>
+      <c r="O98" t="inlineStr"/>
+      <c r="P98" t="inlineStr"/>
     </row>
     <row r="99">
       <c r="A99" t="inlineStr">
         <is>
-          <t>com.chaos.customer</t>
+          <t>com.zwcode.antaivision</t>
         </is>
       </c>
       <c r="B99" t="inlineStr"/>
-      <c r="C99" t="inlineStr"/>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>com.evgvin.feedster</t>
+        </is>
+      </c>
       <c r="D99" t="inlineStr"/>
       <c r="E99" t="inlineStr"/>
+      <c r="F99" t="inlineStr"/>
+      <c r="G99" t="inlineStr"/>
+      <c r="H99" t="inlineStr"/>
+      <c r="I99" t="inlineStr"/>
+      <c r="J99" t="inlineStr"/>
+      <c r="K99" t="inlineStr"/>
+      <c r="L99" t="inlineStr"/>
+      <c r="M99" t="inlineStr"/>
+      <c r="N99" t="inlineStr"/>
+      <c r="O99" t="inlineStr"/>
+      <c r="P99" t="inlineStr"/>
     </row>
     <row r="100">
       <c r="A100" t="inlineStr">
         <is>
-          <t>com.weiou.weiou</t>
+          <t>com.winter.scribble</t>
         </is>
       </c>
       <c r="B100" t="inlineStr"/>
-      <c r="C100" t="inlineStr"/>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>be.rossel.lardennais</t>
+        </is>
+      </c>
       <c r="D100" t="inlineStr"/>
       <c r="E100" t="inlineStr"/>
+      <c r="F100" t="inlineStr"/>
+      <c r="G100" t="inlineStr"/>
+      <c r="H100" t="inlineStr"/>
+      <c r="I100" t="inlineStr"/>
+      <c r="J100" t="inlineStr"/>
+      <c r="K100" t="inlineStr"/>
+      <c r="L100" t="inlineStr"/>
+      <c r="M100" t="inlineStr"/>
+      <c r="N100" t="inlineStr"/>
+      <c r="O100" t="inlineStr"/>
+      <c r="P100" t="inlineStr"/>
     </row>
     <row r="101">
       <c r="A101" t="inlineStr">
         <is>
-          <t>com.q1.juicyhit</t>
+          <t>com.yousgame.MyAnimalIslandU6</t>
         </is>
       </c>
       <c r="B101" t="inlineStr"/>
-      <c r="C101" t="inlineStr"/>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>com.audaxis.mobile.smart.union</t>
+        </is>
+      </c>
       <c r="D101" t="inlineStr"/>
       <c r="E101" t="inlineStr"/>
+      <c r="F101" t="inlineStr"/>
+      <c r="G101" t="inlineStr"/>
+      <c r="H101" t="inlineStr"/>
+      <c r="I101" t="inlineStr"/>
+      <c r="J101" t="inlineStr"/>
+      <c r="K101" t="inlineStr"/>
+      <c r="L101" t="inlineStr"/>
+      <c r="M101" t="inlineStr"/>
+      <c r="N101" t="inlineStr"/>
+      <c r="O101" t="inlineStr"/>
+      <c r="P101" t="inlineStr"/>
     </row>
     <row r="102">
       <c r="A102" t="inlineStr">
         <is>
-          <t>Don't Tap The White Tile_4.0.7.5_apkcombo.com</t>
+          <t>com.uantronic.goshop3d</t>
         </is>
       </c>
       <c r="B102" t="inlineStr"/>
-      <c r="C102" t="inlineStr"/>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>com.videoeditor.videomaker.photos.music.pictures</t>
+        </is>
+      </c>
       <c r="D102" t="inlineStr"/>
       <c r="E102" t="inlineStr"/>
+      <c r="F102" t="inlineStr"/>
+      <c r="G102" t="inlineStr"/>
+      <c r="H102" t="inlineStr"/>
+      <c r="I102" t="inlineStr"/>
+      <c r="J102" t="inlineStr"/>
+      <c r="K102" t="inlineStr"/>
+      <c r="L102" t="inlineStr"/>
+      <c r="M102" t="inlineStr"/>
+      <c r="N102" t="inlineStr"/>
+      <c r="O102" t="inlineStr"/>
+      <c r="P102" t="inlineStr"/>
     </row>
     <row r="103">
       <c r="A103" t="inlineStr">
         <is>
-          <t>com.zhong.mac.fetalheartapp</t>
+          <t>com.wakeup.weikefit</t>
         </is>
       </c>
       <c r="B103" t="inlineStr"/>
-      <c r="C103" t="inlineStr"/>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>com.centaline.centalinemacau</t>
+        </is>
+      </c>
       <c r="D103" t="inlineStr"/>
       <c r="E103" t="inlineStr"/>
+      <c r="F103" t="inlineStr"/>
+      <c r="G103" t="inlineStr"/>
+      <c r="H103" t="inlineStr"/>
+      <c r="I103" t="inlineStr"/>
+      <c r="J103" t="inlineStr"/>
+      <c r="K103" t="inlineStr"/>
+      <c r="L103" t="inlineStr"/>
+      <c r="M103" t="inlineStr"/>
+      <c r="N103" t="inlineStr"/>
+      <c r="O103" t="inlineStr"/>
+      <c r="P103" t="inlineStr"/>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr"/>
+      <c r="B104" t="inlineStr"/>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>cat.gencat.mobi.rodalies</t>
+        </is>
+      </c>
+      <c r="D104" t="inlineStr"/>
+      <c r="E104" t="inlineStr"/>
+      <c r="F104" t="inlineStr"/>
+      <c r="G104" t="inlineStr"/>
+      <c r="H104" t="inlineStr"/>
+      <c r="I104" t="inlineStr"/>
+      <c r="J104" t="inlineStr"/>
+      <c r="K104" t="inlineStr"/>
+      <c r="L104" t="inlineStr"/>
+      <c r="M104" t="inlineStr"/>
+      <c r="N104" t="inlineStr"/>
+      <c r="O104" t="inlineStr"/>
+      <c r="P104" t="inlineStr"/>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr"/>
+      <c r="B105" t="inlineStr"/>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>com.urmet.bv.bvcloudpro</t>
+        </is>
+      </c>
+      <c r="D105" t="inlineStr"/>
+      <c r="E105" t="inlineStr"/>
+      <c r="F105" t="inlineStr"/>
+      <c r="G105" t="inlineStr"/>
+      <c r="H105" t="inlineStr"/>
+      <c r="I105" t="inlineStr"/>
+      <c r="J105" t="inlineStr"/>
+      <c r="K105" t="inlineStr"/>
+      <c r="L105" t="inlineStr"/>
+      <c r="M105" t="inlineStr"/>
+      <c r="N105" t="inlineStr"/>
+      <c r="O105" t="inlineStr"/>
+      <c r="P105" t="inlineStr"/>
+    </row>
+    <row r="106">
+      <c r="A106" t="inlineStr"/>
+      <c r="B106" t="inlineStr"/>
+      <c r="C106" t="inlineStr">
+        <is>
+          <t>com.ce.gwadarpro</t>
+        </is>
+      </c>
+      <c r="D106" t="inlineStr"/>
+      <c r="E106" t="inlineStr"/>
+      <c r="F106" t="inlineStr"/>
+      <c r="G106" t="inlineStr"/>
+      <c r="H106" t="inlineStr"/>
+      <c r="I106" t="inlineStr"/>
+      <c r="J106" t="inlineStr"/>
+      <c r="K106" t="inlineStr"/>
+      <c r="L106" t="inlineStr"/>
+      <c r="M106" t="inlineStr"/>
+      <c r="N106" t="inlineStr"/>
+      <c r="O106" t="inlineStr"/>
+      <c r="P106" t="inlineStr"/>
+    </row>
+    <row r="107">
+      <c r="A107" t="inlineStr"/>
+      <c r="B107" t="inlineStr"/>
+      <c r="C107" t="inlineStr">
+        <is>
+          <t>com.zjw.wearhealth</t>
+        </is>
+      </c>
+      <c r="D107" t="inlineStr"/>
+      <c r="E107" t="inlineStr"/>
+      <c r="F107" t="inlineStr"/>
+      <c r="G107" t="inlineStr"/>
+      <c r="H107" t="inlineStr"/>
+      <c r="I107" t="inlineStr"/>
+      <c r="J107" t="inlineStr"/>
+      <c r="K107" t="inlineStr"/>
+      <c r="L107" t="inlineStr"/>
+      <c r="M107" t="inlineStr"/>
+      <c r="N107" t="inlineStr"/>
+      <c r="O107" t="inlineStr"/>
+      <c r="P107" t="inlineStr"/>
+    </row>
+    <row r="108">
+      <c r="A108" t="inlineStr"/>
+      <c r="B108" t="inlineStr"/>
+      <c r="C108" t="inlineStr">
+        <is>
+          <t>com.snoppa.Snoppa</t>
+        </is>
+      </c>
+      <c r="D108" t="inlineStr"/>
+      <c r="E108" t="inlineStr"/>
+      <c r="F108" t="inlineStr"/>
+      <c r="G108" t="inlineStr"/>
+      <c r="H108" t="inlineStr"/>
+      <c r="I108" t="inlineStr"/>
+      <c r="J108" t="inlineStr"/>
+      <c r="K108" t="inlineStr"/>
+      <c r="L108" t="inlineStr"/>
+      <c r="M108" t="inlineStr"/>
+      <c r="N108" t="inlineStr"/>
+      <c r="O108" t="inlineStr"/>
+      <c r="P108" t="inlineStr"/>
+    </row>
+    <row r="109">
+      <c r="A109" t="inlineStr"/>
+      <c r="B109" t="inlineStr"/>
+      <c r="C109" t="inlineStr">
+        <is>
+          <t>com.accor.appli.hybrid</t>
+        </is>
+      </c>
+      <c r="D109" t="inlineStr"/>
+      <c r="E109" t="inlineStr"/>
+      <c r="F109" t="inlineStr"/>
+      <c r="G109" t="inlineStr"/>
+      <c r="H109" t="inlineStr"/>
+      <c r="I109" t="inlineStr"/>
+      <c r="J109" t="inlineStr"/>
+      <c r="K109" t="inlineStr"/>
+      <c r="L109" t="inlineStr"/>
+      <c r="M109" t="inlineStr"/>
+      <c r="N109" t="inlineStr"/>
+      <c r="O109" t="inlineStr"/>
+      <c r="P109" t="inlineStr"/>
+    </row>
+    <row r="110">
+      <c r="A110" t="inlineStr"/>
+      <c r="B110" t="inlineStr"/>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>com.audaxis.mobile.sudpresse.lanouvellegazette</t>
+        </is>
+      </c>
+      <c r="D110" t="inlineStr"/>
+      <c r="E110" t="inlineStr"/>
+      <c r="F110" t="inlineStr"/>
+      <c r="G110" t="inlineStr"/>
+      <c r="H110" t="inlineStr"/>
+      <c r="I110" t="inlineStr"/>
+      <c r="J110" t="inlineStr"/>
+      <c r="K110" t="inlineStr"/>
+      <c r="L110" t="inlineStr"/>
+      <c r="M110" t="inlineStr"/>
+      <c r="N110" t="inlineStr"/>
+      <c r="O110" t="inlineStr"/>
+      <c r="P110" t="inlineStr"/>
+    </row>
+    <row r="111">
+      <c r="A111" t="inlineStr"/>
+      <c r="B111" t="inlineStr"/>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>com.fgl.adrianmarik.anastasiaroseflowerprincessfree</t>
+        </is>
+      </c>
+      <c r="D111" t="inlineStr"/>
+      <c r="E111" t="inlineStr"/>
+      <c r="F111" t="inlineStr"/>
+      <c r="G111" t="inlineStr"/>
+      <c r="H111" t="inlineStr"/>
+      <c r="I111" t="inlineStr"/>
+      <c r="J111" t="inlineStr"/>
+      <c r="K111" t="inlineStr"/>
+      <c r="L111" t="inlineStr"/>
+      <c r="M111" t="inlineStr"/>
+      <c r="N111" t="inlineStr"/>
+      <c r="O111" t="inlineStr"/>
+      <c r="P111" t="inlineStr"/>
+    </row>
+    <row r="112">
+      <c r="A112" t="inlineStr"/>
+      <c r="B112" t="inlineStr"/>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>Spotify_8.8.88.397_apkcombo.com</t>
+        </is>
+      </c>
+      <c r="D112" t="inlineStr"/>
+      <c r="E112" t="inlineStr"/>
+      <c r="F112" t="inlineStr"/>
+      <c r="G112" t="inlineStr"/>
+      <c r="H112" t="inlineStr"/>
+      <c r="I112" t="inlineStr"/>
+      <c r="J112" t="inlineStr"/>
+      <c r="K112" t="inlineStr"/>
+      <c r="L112" t="inlineStr"/>
+      <c r="M112" t="inlineStr"/>
+      <c r="N112" t="inlineStr"/>
+      <c r="O112" t="inlineStr"/>
+      <c r="P112" t="inlineStr"/>
+    </row>
+    <row r="113">
+      <c r="A113" t="inlineStr"/>
+      <c r="B113" t="inlineStr"/>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>com.zwcode.antaivision</t>
+        </is>
+      </c>
+      <c r="D113" t="inlineStr"/>
+      <c r="E113" t="inlineStr"/>
+      <c r="F113" t="inlineStr"/>
+      <c r="G113" t="inlineStr"/>
+      <c r="H113" t="inlineStr"/>
+      <c r="I113" t="inlineStr"/>
+      <c r="J113" t="inlineStr"/>
+      <c r="K113" t="inlineStr"/>
+      <c r="L113" t="inlineStr"/>
+      <c r="M113" t="inlineStr"/>
+      <c r="N113" t="inlineStr"/>
+      <c r="O113" t="inlineStr"/>
+      <c r="P113" t="inlineStr"/>
+    </row>
+    <row r="114">
+      <c r="A114" t="inlineStr"/>
+      <c r="B114" t="inlineStr"/>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>com.app.aircaraibes</t>
+        </is>
+      </c>
+      <c r="D114" t="inlineStr"/>
+      <c r="E114" t="inlineStr"/>
+      <c r="F114" t="inlineStr"/>
+      <c r="G114" t="inlineStr"/>
+      <c r="H114" t="inlineStr"/>
+      <c r="I114" t="inlineStr"/>
+      <c r="J114" t="inlineStr"/>
+      <c r="K114" t="inlineStr"/>
+      <c r="L114" t="inlineStr"/>
+      <c r="M114" t="inlineStr"/>
+      <c r="N114" t="inlineStr"/>
+      <c r="O114" t="inlineStr"/>
+      <c r="P114" t="inlineStr"/>
+    </row>
+    <row r="115">
+      <c r="A115" t="inlineStr"/>
+      <c r="B115" t="inlineStr"/>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>com.FidgetSpinnerinSpace.starrapps</t>
+        </is>
+      </c>
+      <c r="D115" t="inlineStr"/>
+      <c r="E115" t="inlineStr"/>
+      <c r="F115" t="inlineStr"/>
+      <c r="G115" t="inlineStr"/>
+      <c r="H115" t="inlineStr"/>
+      <c r="I115" t="inlineStr"/>
+      <c r="J115" t="inlineStr"/>
+      <c r="K115" t="inlineStr"/>
+      <c r="L115" t="inlineStr"/>
+      <c r="M115" t="inlineStr"/>
+      <c r="N115" t="inlineStr"/>
+      <c r="O115" t="inlineStr"/>
+      <c r="P115" t="inlineStr"/>
+    </row>
+    <row r="116">
+      <c r="A116" t="inlineStr"/>
+      <c r="B116" t="inlineStr"/>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>com.x10_linked.cam</t>
+        </is>
+      </c>
+      <c r="D116" t="inlineStr"/>
+      <c r="E116" t="inlineStr"/>
+      <c r="F116" t="inlineStr"/>
+      <c r="G116" t="inlineStr"/>
+      <c r="H116" t="inlineStr"/>
+      <c r="I116" t="inlineStr"/>
+      <c r="J116" t="inlineStr"/>
+      <c r="K116" t="inlineStr"/>
+      <c r="L116" t="inlineStr"/>
+      <c r="M116" t="inlineStr"/>
+      <c r="N116" t="inlineStr"/>
+      <c r="O116" t="inlineStr"/>
+      <c r="P116" t="inlineStr"/>
+    </row>
+    <row r="117">
+      <c r="A117" t="inlineStr"/>
+      <c r="B117" t="inlineStr"/>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>com.tkl.fitup</t>
+        </is>
+      </c>
+      <c r="D117" t="inlineStr"/>
+      <c r="E117" t="inlineStr"/>
+      <c r="F117" t="inlineStr"/>
+      <c r="G117" t="inlineStr"/>
+      <c r="H117" t="inlineStr"/>
+      <c r="I117" t="inlineStr"/>
+      <c r="J117" t="inlineStr"/>
+      <c r="K117" t="inlineStr"/>
+      <c r="L117" t="inlineStr"/>
+      <c r="M117" t="inlineStr"/>
+      <c r="N117" t="inlineStr"/>
+      <c r="O117" t="inlineStr"/>
+      <c r="P117" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>